<commit_message>
system_overview.xlsx revision. util/UnifyDataset.py placeholder scriptadded. PredictYOLOv3.py script added.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A10178-40C4-4B4E-92F2-CD1ECA2F0E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341D0B0B-5203-470F-AA44-0D96D511E820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -702,11 +702,20 @@
     <t xml:space="preserve">The system shall come with fully functional scripts for aquiring relevant data for the training of CNN neural network in form of python scripts using data from CARLA simulator. Including scripts for generating .csv file with relevant data, unification of relevant .csv files in .csv for training purposes of CNN neural network. </t>
   </si>
   <si>
-    <t>aquiring script: ./yolov3/?.py
-unification script: ./util/?.py</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>aquiring script: ./yolov3/PredictYOLOv3.py
+unification script: ./util/UnifyDataset.py</t>
+  </si>
+  <si>
+    <t>Code across the project shall have uniform naming convention.</t>
+  </si>
+  <si>
+    <t>Code across the project shall have uniform predetermined naming convention.</t>
+  </si>
+  <si>
+    <t>camelCase</t>
   </si>
 </sst>
 </file>
@@ -896,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1125,6 +1134,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1443,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:P23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,17 +2158,21 @@
       </c>
       <c r="P23" s="30"/>
       <c r="Q23" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>112</v>
+      </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -2168,9 +2184,13 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="25"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="21"/>
+      <c r="O24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="80" t="s">
+        <v>113</v>
+      </c>
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
     </row>
@@ -2722,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -2787,7 +2807,7 @@
       </c>
       <c r="N2" s="73"/>
       <c r="O2" s="78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P2" s="60" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
FUN-ID-21: Script for aquiring data relevant data from YOLOv3 finished. Work done on UnifyDataset.py, yolov3/cfg/coco.names added.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341D0B0B-5203-470F-AA44-0D96D511E820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB6271F-1288-47B1-8A78-9859F94F5426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -958,22 +958,72 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -983,16 +1033,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,25 +1051,41 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1043,100 +1106,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1456,7 +1456,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="O23" sqref="O23:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,27 +1469,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1498,29 +1498,29 @@
       <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="40" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="40" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="41"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="34"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1529,29 +1529,29 @@
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="31" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="22" t="s">
+      <c r="P3" s="30"/>
+      <c r="Q3" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -1560,29 +1560,29 @@
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="29" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="21" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -1591,29 +1591,29 @@
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="29" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="22" t="s">
+      <c r="P5" s="36"/>
+      <c r="Q5" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1622,29 +1622,29 @@
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="29" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="21" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1653,27 +1653,27 @@
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="31" t="s">
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1682,29 +1682,29 @@
       <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="29" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="21" t="s">
+      <c r="P8" s="36"/>
+      <c r="Q8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -1713,27 +1713,27 @@
       <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="31" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1742,29 +1742,29 @@
       <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="29" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="21" t="s">
+      <c r="P10" s="36"/>
+      <c r="Q10" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -1773,27 +1773,27 @@
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="31" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -1802,29 +1802,29 @@
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="34" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="33" t="s">
+      <c r="P12" s="50"/>
+      <c r="Q12" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1833,27 +1833,27 @@
       <c r="B13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="29" t="s">
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -1862,27 +1862,27 @@
       <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="31" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1891,29 +1891,29 @@
       <c r="B15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="31" t="s">
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="22" t="s">
+      <c r="P15" s="30"/>
+      <c r="Q15" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -1922,29 +1922,29 @@
       <c r="B16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="31" t="s">
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="21" t="s">
+      <c r="P16" s="30"/>
+      <c r="Q16" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1953,29 +1953,29 @@
       <c r="B17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="31" t="s">
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="22" t="s">
+      <c r="P17" s="30"/>
+      <c r="Q17" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -1984,29 +1984,29 @@
       <c r="B18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="31" t="s">
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="21" t="s">
+      <c r="P18" s="30"/>
+      <c r="Q18" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -2015,29 +2015,29 @@
       <c r="B19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="29" t="s">
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="22" t="s">
+      <c r="P19" s="36"/>
+      <c r="Q19" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -2046,29 +2046,29 @@
       <c r="B20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="29" t="s">
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="21" t="s">
+      <c r="P20" s="36"/>
+      <c r="Q20" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -2077,29 +2077,29 @@
       <c r="B21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="29" t="s">
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="22" t="s">
+      <c r="P21" s="36"/>
+      <c r="Q21" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -2108,29 +2108,29 @@
       <c r="B22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="31" t="s">
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="21" t="s">
+      <c r="P22" s="30"/>
+      <c r="Q22" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -2139,29 +2139,29 @@
       <c r="B23" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="22" t="s">
+      <c r="P23" s="50"/>
+      <c r="Q23" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -2170,51 +2170,108 @@
       <c r="B24" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="29" t="s">
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="80" t="s">
+      <c r="P24" s="50"/>
+      <c r="Q24" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="C25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="C23:N23"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="Q14:S14"/>
@@ -2231,63 +2288,6 @@
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="C25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="C23:N23"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2310,62 +2310,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="26" t="s">
         <v>103</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="42" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="56" t="s">
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -2377,29 +2377,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="22" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="26" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="54"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="58"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2411,29 +2411,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="36" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="51" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2445,29 +2445,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46" t="s">
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="52" t="s">
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2479,29 +2479,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="36" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="51" t="s">
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="51"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -2513,29 +2513,29 @@
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="46" t="s">
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="52" t="s">
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -2547,29 +2547,29 @@
       <c r="C8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="36" t="s">
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="51" t="s">
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -2581,50 +2581,50 @@
       <c r="C9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46" t="s">
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="52" t="s">
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -2704,6 +2704,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -2720,18 +2732,6 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2754,28 +2754,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2784,38 +2784,38 @@
       <c r="B2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="60" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="39" t="s">
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39" t="s">
+      <c r="J2" s="31"/>
+      <c r="K2" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="60" t="s">
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="73"/>
-      <c r="O2" s="78" t="s">
+      <c r="N2" s="76"/>
+      <c r="O2" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="P2" s="60" t="s">
+      <c r="P2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="61"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="79"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -2829,38 +2829,38 @@
       <c r="B3" s="14">
         <v>4045</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="70">
         <v>5</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="64" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="64" t="s">
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="67"/>
-      <c r="K3" s="69" t="s">
+      <c r="J3" s="71"/>
+      <c r="K3" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="69" t="s">
+      <c r="L3" s="74"/>
+      <c r="M3" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="79" t="s">
+      <c r="N3" s="74"/>
+      <c r="O3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="67"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="71"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -2871,25 +2871,25 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="38"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="47"/>
       <c r="O4" s="15"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="38"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="47"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -2900,25 +2900,25 @@
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="76"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="25"/>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
@@ -2929,25 +2929,25 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="38"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="47"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="38"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="47"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -2958,25 +2958,25 @@
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="76"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="25"/>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -2987,25 +2987,25 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="38"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="47"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="38"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3016,25 +3016,25 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="71"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="76"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="25"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -3045,73 +3045,73 @@
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="38"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="47"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="38"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="47"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="76"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="25"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="38"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="47"/>
       <c r="O12" s="15"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="38"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="47"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -3178,30 +3178,27 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K2:L2"/>
@@ -3218,29 +3215,32 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
system_overview.xslx - new CNN parameters added. UnifyDataset.py - constructs training ready .csv file. PredictYOLOv3.py - path to dataset update.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB6271F-1288-47B1-8A78-9859F94F5426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCBFC1D-6C85-468B-A51D-A710EC7ADB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="117">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Vehicles are present on the current image</t>
   </si>
   <si>
-    <t>Size is debatable. Do we need whole image for the lane processing?</t>
-  </si>
-  <si>
     <t>Functional overview</t>
   </si>
   <si>
@@ -547,14 +544,123 @@
     <t>1280x720 pixels normalized to the range [0, 255] and resized to input dimensions of CNN 100x100 pixels</t>
   </si>
   <si>
-    <t>Veicles present in adjecent lanes of driving lane</t>
-  </si>
-  <si>
-    <t>Describes that there are vehicles in adject lanes relative to the driving lane</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0 - Vehicles present in adjecent lanes
+    <r>
+      <t xml:space="preserve">This parameter is in corelation to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CNN parameter ID-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Related to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CNN parameter ID-4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> To be determined if necessary.</t>
+    </r>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>CNN training overview</t>
+  </si>
+  <si>
+    <t>Dataset size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outputs of CNN </t>
+  </si>
+  <si>
+    <t>CNN parameters used</t>
+  </si>
+  <si>
+    <t>Training accuracy</t>
+  </si>
+  <si>
+    <t>Validation accuracy</t>
+  </si>
+  <si>
+    <t>Test validation acc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>Minimal set of parameters used for determining the successfulness of the CNN to be used in the system.</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional scripts for aquiring relevant data for the training of CNN neural network.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall come with fully functional scripts for aquiring relevant data for the training of CNN neural network in form of python scripts using data from CARLA simulator. Including scripts for generating .csv file with relevant data, unification of relevant .csv files in .csv for training purposes of CNN neural network. </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>aquiring script: ./yolov3/PredictYOLOv3.py
+unification script: ./util/UnifyDataset.py</t>
+  </si>
+  <si>
+    <t>Code across the project shall have uniform naming convention.</t>
+  </si>
+  <si>
+    <t>Code across the project shall have uniform predetermined naming convention.</t>
+  </si>
+  <si>
+    <t>camelCase</t>
+  </si>
+  <si>
+    <t>Veicles present in the left lane of driving lane</t>
+  </si>
+  <si>
+    <t>Veicles present in the right lane of driving lane</t>
+  </si>
+  <si>
+    <t>Describes that there are vehicles in adject left lane relative to the driving lane</t>
+  </si>
+  <si>
+    <t>Describes that there are vehicles in adject right lane relative to the driving lane</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 - Vehicles present in adjecent left lane
 1 - Vehicles </t>
     </r>
     <r>
@@ -576,12 +682,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> present in adjecent lanes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This parameter is in corelation to the </t>
+      <t xml:space="preserve"> present in adjecent left lane</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 - Vehicles present in adjecent right lane
+1 - Vehicles </t>
     </r>
     <r>
       <rPr>
@@ -592,7 +699,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CNN parameter ID-2</t>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> present in adjecent right lane</t>
+    </r>
+  </si>
+  <si>
+    <t>ID-2, ID-3, ID-5, ID-7, ID-8</t>
+  </si>
+  <si>
+    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Related to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CNN parameter ID-7, ID-8.</t>
     </r>
   </si>
   <si>
@@ -610,22 +749,6 @@
       </rPr>
       <t>CNN parameter ID-2, ID-6, ID-7</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Related to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CNN parameter ID-4.</t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -634,95 +757,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> To be determined if necessary.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Related to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CNN parameter ID-7.</t>
-    </r>
-  </si>
-  <si>
-    <t>Iteration</t>
-  </si>
-  <si>
-    <t>CNN training overview</t>
-  </si>
-  <si>
-    <t>Dataset size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outputs of CNN </t>
-  </si>
-  <si>
-    <t>CNN parameters used</t>
-  </si>
-  <si>
-    <t>Training accuracy</t>
-  </si>
-  <si>
-    <t>Validation accuracy</t>
-  </si>
-  <si>
-    <t>Test validation acc</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>ID-2, ID-3, ID-5, ID-6, ID-7</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
-    <t>Minimal set of parameters used for determining the successfulness of the CNN to be used in the system.</t>
-  </si>
-  <si>
-    <t>The system shall come with fully functional scripts for aquiring relevant data for the training of CNN neural network.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system shall come with fully functional scripts for aquiring relevant data for the training of CNN neural network in form of python scripts using data from CARLA simulator. Including scripts for generating .csv file with relevant data, unification of relevant .csv files in .csv for training purposes of CNN neural network. </t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>aquiring script: ./yolov3/PredictYOLOv3.py
-unification script: ./util/UnifyDataset.py</t>
-  </si>
-  <si>
-    <t>Code across the project shall have uniform naming convention.</t>
-  </si>
-  <si>
-    <t>Code across the project shall have uniform predetermined naming convention.</t>
-  </si>
-  <si>
-    <t>camelCase</t>
+      <t>, ID-8</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,6 +785,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -905,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -941,7 +990,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -985,6 +1033,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1124,20 +1176,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1455,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:P23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,749 +1521,749 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="33" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="34"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="35"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
+        <v>33</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
+      <c r="C5" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
+      <c r="C15" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
+        <v>76</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
+      <c r="B23" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="R23" s="42"/>
+      <c r="S23" s="42"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
+      <c r="B24" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="73">
@@ -2299,334 +2351,347 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="16"/>
+    <col min="2" max="2" width="9.140625" style="15"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="15" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>103</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>96</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="40" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="60" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="58"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="45" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="55" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="67" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="56" t="s">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="45" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="55" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="67" t="s">
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="56" t="s">
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="55" t="s">
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="56"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="51"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+    </row>
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+    </row>
+    <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -2645,7 +2710,7 @@
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -2733,6 +2798,7 @@
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2740,82 +2806,82 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="16"/>
+    <col min="15" max="15" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="78"/>
+      <c r="E2" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="75" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2" s="75" t="s">
+      <c r="L2" s="80"/>
+      <c r="M2" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="81"/>
+      <c r="O2" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="P2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="79"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="78"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -2826,41 +2892,41 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>4045</v>
       </c>
-      <c r="C3" s="70">
+      <c r="C3" s="71">
         <v>5</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="70" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="74"/>
-      <c r="M3" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="71"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="72"/>
+      <c r="K3" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="75"/>
+      <c r="M3" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="75"/>
+      <c r="O3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="72"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -2871,25 +2937,25 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="47"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="48"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -2900,25 +2966,25 @@
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="25"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="24"/>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
@@ -2929,25 +2995,25 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="47"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="48"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -2958,25 +3024,25 @@
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="25"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="24"/>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -2987,25 +3053,25 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="47"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="48"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3016,25 +3082,25 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="24"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -3045,136 +3111,139 @@
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="47"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="48"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="24"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="47"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="48"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F16" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="63">
@@ -3184,9 +3253,13 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="P8:T8"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -3194,39 +3267,33 @@
     <mergeCell ref="P6:T6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="P4:T4"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="P12:T12"/>
@@ -3241,6 +3308,8 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bugfixes and preparation for first iteration of training of the CNN model.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCBFC1D-6C85-468B-A51D-A710EC7ADB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A5D895-512D-4BD6-B787-C43C5938411F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -1037,74 +1037,92 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,53 +1158,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1507,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7:S7"/>
     </sheetView>
   </sheetViews>
@@ -1521,27 +1521,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1550,29 +1550,29 @@
       <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="34" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="34" t="s">
+      <c r="P2" s="52"/>
+      <c r="Q2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="41"/>
-      <c r="S2" s="35"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="52"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1581,29 +1581,29 @@
       <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="30" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="42" t="s">
+      <c r="P3" s="45"/>
+      <c r="Q3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -1612,29 +1612,29 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="36" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="33" t="s">
+      <c r="P4" s="43"/>
+      <c r="Q4" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -1643,29 +1643,29 @@
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="36" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="42" t="s">
+      <c r="P5" s="43"/>
+      <c r="Q5" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1674,29 +1674,29 @@
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="36" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="33" t="s">
+      <c r="P6" s="43"/>
+      <c r="Q6" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1705,27 +1705,27 @@
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="30" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1734,29 +1734,29 @@
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="36" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="33" t="s">
+      <c r="P8" s="43"/>
+      <c r="Q8" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -1765,27 +1765,27 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="30" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1794,29 +1794,29 @@
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="36" t="s">
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="33" t="s">
+      <c r="P10" s="43"/>
+      <c r="Q10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -1825,27 +1825,27 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="30" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -1854,29 +1854,29 @@
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="50" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="49" t="s">
+      <c r="P12" s="37"/>
+      <c r="Q12" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="R12" s="33"/>
-      <c r="S12" s="33"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1885,27 +1885,27 @@
       <c r="B13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="36" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -1914,27 +1914,27 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="30" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1943,29 +1943,29 @@
       <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="30" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="42" t="s">
+      <c r="P15" s="45"/>
+      <c r="Q15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -1974,29 +1974,29 @@
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="30" t="s">
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="33" t="s">
+      <c r="P16" s="45"/>
+      <c r="Q16" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -2005,29 +2005,29 @@
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="30" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="42" t="s">
+      <c r="P17" s="45"/>
+      <c r="Q17" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -2036,29 +2036,29 @@
       <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="30" t="s">
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="33" t="s">
+      <c r="P18" s="45"/>
+      <c r="Q18" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -2067,29 +2067,29 @@
       <c r="B19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="36" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="42" t="s">
+      <c r="P19" s="43"/>
+      <c r="Q19" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -2098,29 +2098,29 @@
       <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="36" t="s">
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="33" t="s">
+      <c r="P20" s="43"/>
+      <c r="Q20" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -2129,29 +2129,29 @@
       <c r="B21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="36" t="s">
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="42" t="s">
+      <c r="P21" s="43"/>
+      <c r="Q21" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -2160,29 +2160,29 @@
       <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="30" t="s">
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="33" t="s">
+      <c r="P22" s="45"/>
+      <c r="Q22" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -2191,29 +2191,29 @@
       <c r="B23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="50" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="42" t="s">
+      <c r="P23" s="37"/>
+      <c r="Q23" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -2222,51 +2222,108 @@
       <c r="B24" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="50" t="s">
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="53" t="s">
+      <c r="P24" s="37"/>
+      <c r="Q24" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="52"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
     <mergeCell ref="C25:N25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:S25"/>
@@ -2283,63 +2340,6 @@
     <mergeCell ref="C23:N23"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="C14:N14"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2362,28 +2362,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2395,29 +2395,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="41" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="61" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -2429,29 +2429,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="42" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="43" t="s">
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="59"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="65"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2463,29 +2463,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="46" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="56" t="s">
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2497,29 +2497,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68" t="s">
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="57" t="s">
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2531,29 +2531,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="46" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="56" t="s">
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -2565,29 +2565,29 @@
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="68" t="s">
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="57" t="s">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -2599,29 +2599,29 @@
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="46" t="s">
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="56" t="s">
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -2633,29 +2633,29 @@
       <c r="C9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="68" t="s">
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="57" t="s">
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -2667,29 +2667,29 @@
       <c r="C10" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="46" t="s">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="56" t="s">
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="56"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -2769,18 +2769,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -2797,6 +2785,18 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2808,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,28 +2820,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2850,38 +2850,38 @@
       <c r="B2" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="76" t="s">
+      <c r="D2" s="73"/>
+      <c r="E2" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="32" t="s">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="76" t="s">
+      <c r="L2" s="79"/>
+      <c r="M2" s="71" t="s">
         <v>94</v>
       </c>
       <c r="N2" s="81"/>
       <c r="O2" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="P2" s="76" t="s">
+      <c r="P2" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="78"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="73"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -2893,40 +2893,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>4045</v>
-      </c>
-      <c r="C3" s="71">
+        <v>1218</v>
+      </c>
+      <c r="C3" s="74">
         <v>5</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="71" t="s">
+      <c r="D3" s="76"/>
+      <c r="E3" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="71" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="72"/>
-      <c r="K3" s="73" t="s">
+      <c r="J3" s="76"/>
+      <c r="K3" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="75"/>
-      <c r="M3" s="73" t="s">
+      <c r="L3" s="78"/>
+      <c r="M3" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="75"/>
+      <c r="N3" s="78"/>
       <c r="O3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="72"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="76"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -2938,24 +2938,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="48"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="49"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="48"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="49"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -2967,18 +2967,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="75"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="78"/>
       <c r="O5" s="20"/>
       <c r="P5" s="19"/>
       <c r="Q5" s="22"/>
@@ -2996,24 +2996,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="48"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="49"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="48"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="49"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -3025,18 +3025,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="75"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="78"/>
       <c r="O7" s="20"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="22"/>
@@ -3054,24 +3054,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="48"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="49"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="48"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="49"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3083,18 +3083,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="75"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="78"/>
       <c r="O9" s="20"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="22"/>
@@ -3112,42 +3112,42 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="48"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="49"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="48"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="49"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="75"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="78"/>
       <c r="O11" s="20"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="22"/>
@@ -3160,24 +3160,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="48"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="49"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="48"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="49"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -3247,37 +3247,21 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:H10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="M10:N10"/>
@@ -3294,22 +3278,38 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CNN model architecture added.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A5D895-512D-4BD6-B787-C43C5938411F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124B2D7B-DD0C-4A26-9B46-AE2D678781D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
     <sheet name="CNN parameters overview" sheetId="1" r:id="rId2"/>
-    <sheet name="CNN training overview" sheetId="3" r:id="rId3"/>
+    <sheet name="CNN architecture overview" sheetId="4" r:id="rId3"/>
+    <sheet name="CNN training overview" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -716,9 +717,6 @@
     <t>ID-2, ID-3, ID-5, ID-7, ID-8</t>
   </si>
   <si>
-    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Related to the </t>
     </r>
@@ -759,6 +757,62 @@
       </rPr>
       <t>, ID-8</t>
     </r>
+  </si>
+  <si>
+    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't
+RoI = 1280 - 0 x 720 - 350 = 1280 x 370 
+Upper 350 pixels in all directions can be removed from the image. Image can be cropped to 1280x370</t>
+  </si>
+  <si>
+    <t>CNN Architecture</t>
+  </si>
+  <si>
+    <t>Input layer</t>
+  </si>
+  <si>
+    <t>100x100</t>
+  </si>
+  <si>
+    <t>Conv2D(16, (3,3), activation= 'relu')</t>
+  </si>
+  <si>
+    <t>Max-pooling layer</t>
+  </si>
+  <si>
+    <t>pool_size = (2, 2)</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>Conv2D(32, (3,3), activation= 'relu')</t>
+  </si>
+  <si>
+    <t>Conv2D(64, (3,3), activation='relu')</t>
+  </si>
+  <si>
+    <t>Flatten</t>
+  </si>
+  <si>
+    <t>Dense layer</t>
+  </si>
+  <si>
+    <t>Convolutive layer</t>
+  </si>
+  <si>
+    <t>Dense(32, activation='relu')</t>
+  </si>
+  <si>
+    <t>Dense(64, activation='relu')</t>
+  </si>
+  <si>
+    <t>Dense(128, activation='relu')</t>
+  </si>
+  <si>
+    <t>output_no</t>
+  </si>
+  <si>
+    <t>To be finaly determined.</t>
   </si>
 </sst>
 </file>
@@ -954,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1037,21 +1091,74 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1059,52 +1166,41 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,38 +1221,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1167,26 +1245,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1521,27 +1584,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1550,29 +1613,29 @@
       <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="51" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="51" t="s">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="52"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="38"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1581,29 +1644,29 @@
       <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="44" t="s">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="32" t="s">
+      <c r="P3" s="34"/>
+      <c r="Q3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -1612,29 +1675,29 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="42" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="31" t="s">
+      <c r="P4" s="40"/>
+      <c r="Q4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -1643,29 +1706,29 @@
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="42" t="s">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="32" t="s">
+      <c r="P5" s="40"/>
+      <c r="Q5" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1674,29 +1737,29 @@
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="42" t="s">
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1705,27 +1768,27 @@
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="44" t="s">
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1734,29 +1797,29 @@
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="42" t="s">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="31" t="s">
+      <c r="P8" s="40"/>
+      <c r="Q8" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -1765,27 +1828,27 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="44" t="s">
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1794,29 +1857,29 @@
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="42" t="s">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="31" t="s">
+      <c r="P10" s="40"/>
+      <c r="Q10" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -1825,27 +1888,27 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="44" t="s">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -1854,29 +1917,29 @@
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="36" t="s">
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="46" t="s">
+      <c r="P12" s="54"/>
+      <c r="Q12" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1885,27 +1948,27 @@
       <c r="B13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="42" t="s">
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -1914,27 +1977,27 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="44" t="s">
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1943,29 +2006,29 @@
       <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="44" t="s">
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="32" t="s">
+      <c r="P15" s="34"/>
+      <c r="Q15" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -1974,29 +2037,29 @@
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="44" t="s">
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="31" t="s">
+      <c r="P16" s="34"/>
+      <c r="Q16" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -2005,29 +2068,29 @@
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="44" t="s">
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="32" t="s">
+      <c r="P17" s="34"/>
+      <c r="Q17" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -2036,29 +2099,29 @@
       <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="44" t="s">
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="31" t="s">
+      <c r="P18" s="34"/>
+      <c r="Q18" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -2067,29 +2130,29 @@
       <c r="B19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="42" t="s">
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="32" t="s">
+      <c r="P19" s="40"/>
+      <c r="Q19" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -2098,29 +2161,29 @@
       <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="42" t="s">
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="31" t="s">
+      <c r="P20" s="40"/>
+      <c r="Q20" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -2129,29 +2192,29 @@
       <c r="B21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="42" t="s">
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -2160,29 +2223,29 @@
       <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="44" t="s">
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="31" t="s">
+      <c r="P22" s="34"/>
+      <c r="Q22" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -2191,29 +2254,29 @@
       <c r="B23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="36" t="s">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="32" t="s">
+      <c r="P23" s="54"/>
+      <c r="Q23" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -2222,51 +2285,108 @@
       <c r="B24" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="36" t="s">
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="38" t="s">
+      <c r="P24" s="54"/>
+      <c r="Q24" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="C25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="C23:N23"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="Q14:S14"/>
@@ -2283,63 +2403,6 @@
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="C25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="C23:N23"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2351,7 +2414,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection sqref="A1:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,28 +2425,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2395,31 +2458,31 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="53" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="67" t="s">
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-    </row>
-    <row r="3" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+    </row>
+    <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -2429,29 +2492,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="32" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="65"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="62"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2463,29 +2526,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="47" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="62" t="s">
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2497,29 +2560,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57" t="s">
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="63" t="s">
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2531,29 +2594,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="47" t="s">
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="62" t="s">
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -2565,29 +2628,29 @@
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="57" t="s">
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="63" t="s">
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -2599,29 +2662,29 @@
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="47" t="s">
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="62" t="s">
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -2633,29 +2696,29 @@
       <c r="C9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="57" t="s">
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="63" t="s">
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -2667,29 +2730,29 @@
       <c r="C10" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="47" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="62" t="s">
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -2769,6 +2832,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -2785,18 +2860,6 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2805,11 +2868,466 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3399D5AB-0FA1-4FE2-AE54-B718FE78F3AD}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="62"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="71">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="71">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="71">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:M3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,28 +3338,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2850,38 +3368,38 @@
       <c r="B2" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="71" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="50" t="s">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50" t="s">
+      <c r="J2" s="35"/>
+      <c r="K2" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="71" t="s">
+      <c r="L2" s="83"/>
+      <c r="M2" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="N2" s="81"/>
+      <c r="N2" s="84"/>
       <c r="O2" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="P2" s="71" t="s">
+      <c r="P2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="73"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -2898,7 +3416,7 @@
       <c r="C3" s="74">
         <v>5</v>
       </c>
-      <c r="D3" s="76"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="74" t="s">
         <v>113</v>
       </c>
@@ -2908,12 +3426,12 @@
       <c r="I3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="76"/>
-      <c r="K3" s="80" t="s">
+      <c r="J3" s="75"/>
+      <c r="K3" s="76" t="s">
         <v>95</v>
       </c>
       <c r="L3" s="78"/>
-      <c r="M3" s="80" t="s">
+      <c r="M3" s="76" t="s">
         <v>95</v>
       </c>
       <c r="N3" s="78"/>
@@ -2923,10 +3441,10 @@
       <c r="P3" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="76"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="75"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -2938,24 +3456,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="51"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="51"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -2968,16 +3486,16 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="74"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="80"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="77"/>
       <c r="G5" s="77"/>
       <c r="H5" s="78"/>
       <c r="I5" s="74"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="80"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
       <c r="L5" s="78"/>
-      <c r="M5" s="80"/>
+      <c r="M5" s="76"/>
       <c r="N5" s="78"/>
       <c r="O5" s="20"/>
       <c r="P5" s="19"/>
@@ -2996,24 +3514,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="51"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="51"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -3026,16 +3544,16 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="74"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="80"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="77"/>
       <c r="G7" s="77"/>
       <c r="H7" s="78"/>
       <c r="I7" s="74"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="80"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="76"/>
       <c r="L7" s="78"/>
-      <c r="M7" s="80"/>
+      <c r="M7" s="76"/>
       <c r="N7" s="78"/>
       <c r="O7" s="20"/>
       <c r="P7" s="19"/>
@@ -3054,24 +3572,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="51"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="51"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3084,16 +3602,16 @@
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="74"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="80"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="76"/>
       <c r="F9" s="77"/>
       <c r="G9" s="77"/>
       <c r="H9" s="78"/>
       <c r="I9" s="74"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="80"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="76"/>
       <c r="L9" s="78"/>
-      <c r="M9" s="80"/>
+      <c r="M9" s="76"/>
       <c r="N9" s="78"/>
       <c r="O9" s="20"/>
       <c r="P9" s="19"/>
@@ -3112,24 +3630,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="51"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="51"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -3137,16 +3655,16 @@
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="74"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="80"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="76"/>
       <c r="F11" s="77"/>
       <c r="G11" s="77"/>
       <c r="H11" s="78"/>
       <c r="I11" s="74"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="80"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
       <c r="L11" s="78"/>
-      <c r="M11" s="80"/>
+      <c r="M11" s="76"/>
       <c r="N11" s="78"/>
       <c r="O11" s="20"/>
       <c r="P11" s="19"/>
@@ -3160,24 +3678,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="51"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="51"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -3247,6 +3765,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="P12:T12"/>
     <mergeCell ref="P10:T10"/>
@@ -3263,53 +3828,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dataset collection process added to system_overview.xlsx
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124B2D7B-DD0C-4A26-9B46-AE2D678781D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC9823C-BEEE-434C-8293-D023A3516FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="4" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
     <sheet name="CNN parameters overview" sheetId="1" r:id="rId2"/>
     <sheet name="CNN architecture overview" sheetId="4" r:id="rId3"/>
     <sheet name="CNN training overview" sheetId="3" r:id="rId4"/>
+    <sheet name="Dataset collection process" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -813,6 +814,15 @@
   </si>
   <si>
     <t>To be finaly determined.</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation in form of python script.</t>
+  </si>
+  <si>
+    <t>./cnn/CNNPredict.py</t>
   </si>
 </sst>
 </file>
@@ -1100,74 +1110,94 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1203,53 +1233,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1269,6 +1281,1160 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161055</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="38" name="Group 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F4DAE9-1B2C-4DA1-B14B-065CBD7E081E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1219200" y="114300"/>
+          <a:ext cx="8696325" cy="3666255"/>
+          <a:chOff x="1771650" y="209550"/>
+          <a:chExt cx="8696325" cy="3666255"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="27" name="Group 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B439411-B979-418A-B830-BE9D3BA034E4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1771650" y="209550"/>
+            <a:ext cx="8696325" cy="3666255"/>
+            <a:chOff x="1200150" y="180975"/>
+            <a:chExt cx="8696325" cy="3666255"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="Rectangle 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167517AA-39AE-4E55-B832-CC4AD2954428}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1200150" y="180975"/>
+              <a:ext cx="8696325" cy="3666255"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3458EFC9-8D34-4F48-A8B1-E41072404D3C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1704975" y="409575"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>Simulation</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data (MainSimulation.py - CNN)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F299CB2D-04D0-4ABE-BA0B-B0FD6E06795F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1762125" y="2171700"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>YOLOv3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF38FEE7-4ABB-463A-A7A6-9DD38C5ACFA3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6324600" y="1333500"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>Unified</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t>(UnifyDataset.py - YOLOv3)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A623ED44-6D0B-43C4-B99F-A2C5230B5890}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="2" idx="3"/>
+              <a:endCxn id="4" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4876800" y="1133475"/>
+              <a:ext cx="1447800" cy="923925"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="57150">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="3">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4495A020-B29D-4DB8-BD65-0BD5497E2A28}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="3" idx="3"/>
+              <a:endCxn id="4" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="4933950" y="2057400"/>
+              <a:ext cx="1390650" cy="838200"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="57150">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="3">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="TextBox 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDBA831F-AFBD-4C4A-BC19-608B08FB727A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6953250" y="333375"/>
+            <a:ext cx="3343275" cy="390525"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="57150" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Dataset collection iteration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>161055</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="Group 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FB9299-223C-433D-8C2E-05123C9240E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1219200" y="5067300"/>
+          <a:ext cx="8696325" cy="3666255"/>
+          <a:chOff x="1771650" y="209550"/>
+          <a:chExt cx="8696325" cy="3666255"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="40" name="Group 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF69B6F-8088-48A5-9544-7ACE4039F940}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1771650" y="209550"/>
+            <a:ext cx="8696325" cy="3666255"/>
+            <a:chOff x="1200150" y="180975"/>
+            <a:chExt cx="8696325" cy="3666255"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="42" name="Rectangle 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBDAA40F-51C2-4E85-8DD8-90CC88835DD6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1200150" y="180975"/>
+              <a:ext cx="8696325" cy="3666255"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315940E0-4DE3-4817-BD25-1E7774B0FDFB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1704975" y="409575"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>Simulation</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data (MainSimulation.py - CNN)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="44" name="Rectangle: Rounded Corners 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D1D8C9-4928-4C24-9014-CDE447855DF4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1762125" y="2171700"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>YOLOv3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="45" name="Rectangle: Rounded Corners 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1897B4CE-C2E4-4F30-BF39-DA0CCE1584E1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6324600" y="1333500"/>
+              <a:ext cx="3171825" cy="1447800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600"/>
+                <a:t>Unified</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t> data</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                <a:t>(UnifyDataset.py - YOLOv3)</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4212E485-8854-4681-A0B9-E18314AA348D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="43" idx="3"/>
+              <a:endCxn id="45" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4876800" y="1133475"/>
+              <a:ext cx="1447800" cy="923925"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="57150">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="3">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F577F37-C557-4212-A3CC-F87973D3A48C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="44" idx="3"/>
+              <a:endCxn id="45" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="4933950" y="2057400"/>
+              <a:ext cx="1390650" cy="838200"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="57150">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="3">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="2">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="41" name="TextBox 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E18763B-4485-4DF1-B23B-827D44DB2401}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6953250" y="333375"/>
+            <a:ext cx="3343275" cy="390525"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="57150" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Dataset collection iteration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t> n</a:t>
+            </a:r>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>598713</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>110506</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>78921</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle: Rounded Corners 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A70677-BE10-46AE-8E1B-0691DABC1FC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12845142" y="2775857"/>
+          <a:ext cx="3185721" cy="3399064"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Combine</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> datasets</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t>(CombineDataset.py - YOLOv3)</a:t>
+          </a:r>
+          <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>372444</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>598713</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>93889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27DE1C-E6CC-4607-9C1D-DD5B646B7362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="50" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9557265" y="1990725"/>
+          <a:ext cx="3287877" cy="2484664"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>372444</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>93889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>598713</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1438C6-9E09-4C18-8732-CDAC98FB0E7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="3"/>
+          <a:endCxn id="50" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9557265" y="4475389"/>
+          <a:ext cx="3287877" cy="2468336"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>110506</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>93889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1275AB8-ACE2-4776-867D-DC3EE92A1925}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="3"/>
+          <a:endCxn id="66" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15960106" y="4467225"/>
+          <a:ext cx="2023094" cy="8164"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Rectangle: Rounded Corners 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD7E897-6210-4864-B6B9-8F42392AAEAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17983200" y="3571875"/>
+          <a:ext cx="1790700" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>FinalDataset.csv</a:t>
+          </a:r>
+          <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1570,8 +2736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:S7"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,27 +2750,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1613,29 +2779,29 @@
       <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="37" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="37" t="s">
+      <c r="P2" s="55"/>
+      <c r="Q2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="38"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="55"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -1644,29 +2810,29 @@
       <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="33" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="45" t="s">
+      <c r="P3" s="48"/>
+      <c r="Q3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -1675,29 +2841,29 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="39" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="46"/>
+      <c r="Q4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -1706,29 +2872,29 @@
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="39" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="45" t="s">
+      <c r="P5" s="46"/>
+      <c r="Q5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1737,29 +2903,29 @@
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="39" t="s">
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="36" t="s">
+      <c r="P6" s="46"/>
+      <c r="Q6" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1768,27 +2934,27 @@
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="33" t="s">
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1797,29 +2963,29 @@
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="39" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="36" t="s">
+      <c r="P8" s="46"/>
+      <c r="Q8" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -1828,27 +2994,27 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="33" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1857,29 +3023,29 @@
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="39" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="36" t="s">
+      <c r="P10" s="46"/>
+      <c r="Q10" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -1888,27 +3054,27 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="33" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -1917,29 +3083,29 @@
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="53" t="s">
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="52" t="s">
+      <c r="P12" s="40"/>
+      <c r="Q12" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1948,27 +3114,27 @@
       <c r="B13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="39" t="s">
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -1977,27 +3143,27 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="33" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -2006,29 +3172,29 @@
       <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="33" t="s">
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="45" t="s">
+      <c r="P15" s="48"/>
+      <c r="Q15" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -2037,29 +3203,29 @@
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="33" t="s">
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="36" t="s">
+      <c r="P16" s="48"/>
+      <c r="Q16" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -2068,29 +3234,29 @@
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="33" t="s">
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="45" t="s">
+      <c r="P17" s="48"/>
+      <c r="Q17" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -2099,29 +3265,29 @@
       <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="33" t="s">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="36" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -2130,29 +3296,29 @@
       <c r="B19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="39" t="s">
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="45" t="s">
+      <c r="P19" s="46"/>
+      <c r="Q19" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -2161,29 +3327,29 @@
       <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="39" t="s">
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="36" t="s">
+      <c r="P20" s="46"/>
+      <c r="Q20" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -2192,29 +3358,29 @@
       <c r="B21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="39" t="s">
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="45" t="s">
+      <c r="P21" s="46"/>
+      <c r="Q21" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -2223,29 +3389,29 @@
       <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="33" t="s">
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="36" t="s">
+      <c r="P22" s="48"/>
+      <c r="Q22" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -2254,29 +3420,29 @@
       <c r="B23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="53" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="45" t="s">
+      <c r="P23" s="40"/>
+      <c r="Q23" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -2285,51 +3451,120 @@
       <c r="B24" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="53" t="s">
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="56" t="s">
+      <c r="P24" s="40"/>
+      <c r="Q24" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55"/>
-      <c r="S25" s="55"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+    </row>
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
     <mergeCell ref="C25:N25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:S25"/>
@@ -2346,63 +3581,6 @@
     <mergeCell ref="C23:N23"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="C14:N14"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2425,28 +3603,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2458,29 +3636,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="44" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="64" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -2492,29 +3670,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="45" t="s">
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="46" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="62"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="68"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2526,29 +3704,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="49" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="59" t="s">
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2560,29 +3738,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71" t="s">
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="60" t="s">
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2594,29 +3772,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="49" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="59" t="s">
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -2628,29 +3806,29 @@
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="71" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="60" t="s">
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -2662,29 +3840,29 @@
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="49" t="s">
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="59" t="s">
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="59"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="59"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -2696,29 +3874,29 @@
       <c r="C9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71" t="s">
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="60" t="s">
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -2730,29 +3908,29 @@
       <c r="C10" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="49" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="59" t="s">
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -2832,18 +4010,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -2860,6 +4026,18 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2871,7 +4049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3399D5AB-0FA1-4FE2-AE54-B718FE78F3AD}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -2881,21 +4059,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2904,21 +4082,21 @@
       <c r="B2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="64" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -2927,19 +4105,19 @@
       <c r="B3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="62"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2948,19 +4126,19 @@
       <c r="B4" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2969,19 +4147,19 @@
       <c r="B5" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -2990,19 +4168,19 @@
       <c r="B6" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="50">
         <v>0.25</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -3011,19 +4189,19 @@
       <c r="B7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -3032,19 +4210,19 @@
       <c r="B8" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -3053,19 +4231,19 @@
       <c r="B9" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="71">
+      <c r="C9" s="60">
         <v>0.25</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -3074,19 +4252,19 @@
       <c r="B10" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -3095,19 +4273,19 @@
       <c r="B11" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -3116,19 +4294,19 @@
       <c r="B12" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="50">
         <v>0.25</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -3137,17 +4315,17 @@
       <c r="B13" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -3156,19 +4334,19 @@
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -3177,19 +4355,19 @@
       <c r="B15" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="71">
+      <c r="C15" s="60">
         <v>0.25</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -3198,19 +4376,19 @@
       <c r="B16" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -3219,19 +4397,19 @@
       <c r="B17" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="71">
+      <c r="C17" s="60">
         <v>0.25</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -3240,19 +4418,19 @@
       <c r="B18" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -3261,52 +4439,24 @@
       <c r="B19" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="60" t="s">
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M7"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="C5:H5"/>
@@ -3316,6 +4466,34 @@
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:M3"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3338,28 +4516,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3368,38 +4546,38 @@
       <c r="B2" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="79" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="35" t="s">
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="79" t="s">
+      <c r="L2" s="82"/>
+      <c r="M2" s="74" t="s">
         <v>94</v>
       </c>
       <c r="N2" s="84"/>
       <c r="O2" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="P2" s="79" t="s">
+      <c r="P2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="76"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
@@ -3413,38 +4591,38 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="74">
+      <c r="C3" s="77">
         <v>5</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="74" t="s">
+      <c r="D3" s="79"/>
+      <c r="E3" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="74" t="s">
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="75"/>
-      <c r="K3" s="76" t="s">
+      <c r="J3" s="79"/>
+      <c r="K3" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="78"/>
-      <c r="M3" s="76" t="s">
+      <c r="L3" s="81"/>
+      <c r="M3" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="78"/>
+      <c r="N3" s="81"/>
       <c r="O3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="74" t="s">
+      <c r="P3" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="75"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="79"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
@@ -3456,24 +4634,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="51"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="52"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="51"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="52"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -3485,18 +4663,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="78"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="81"/>
       <c r="O5" s="20"/>
       <c r="P5" s="19"/>
       <c r="Q5" s="22"/>
@@ -3514,24 +4692,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="51"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="52"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="51"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -3543,18 +4721,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="78"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="81"/>
       <c r="O7" s="20"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="22"/>
@@ -3572,24 +4750,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="51"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="52"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="51"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="52"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3601,18 +4779,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="78"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="81"/>
       <c r="O9" s="20"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="22"/>
@@ -3630,42 +4808,42 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="51"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="52"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="51"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="52"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="78"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="81"/>
       <c r="O11" s="20"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="22"/>
@@ -3678,24 +4856,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="51"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="52"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="51"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="52"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -3765,6 +4943,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P2:T2"/>
@@ -3781,55 +5006,23 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E59531-0B66-425B-ACD4-E8D6EFFE2FF5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD39" sqref="AD39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
system_overview.xlsx Dataset collection process update.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC9823C-BEEE-434C-8293-D023A3516FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63028A40-32F5-4BEF-9FE3-A2B6FDC9AE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="4" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -1311,8 +1311,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1219200" y="114300"/>
-          <a:ext cx="8696325" cy="3666255"/>
+          <a:off x="1212273" y="114300"/>
+          <a:ext cx="8647834" cy="3666255"/>
           <a:chOff x="1771650" y="209550"/>
           <a:chExt cx="8696325" cy="3666255"/>
         </a:xfrm>
@@ -1710,14 +1710,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>127908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>161055</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>174663</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1732,8 +1732,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1219200" y="5067300"/>
-          <a:ext cx="8696325" cy="3666255"/>
+          <a:off x="1212273" y="7557408"/>
+          <a:ext cx="8647834" cy="3666255"/>
           <a:chOff x="1771650" y="209550"/>
           <a:chExt cx="8696325" cy="3666255"/>
         </a:xfrm>
@@ -2131,14 +2131,14 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>110506</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>78921</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2153,7 +2153,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12845142" y="2775857"/>
+          <a:off x="12845142" y="3878036"/>
           <a:ext cx="3185721" cy="3399064"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2212,8 +2212,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>93889</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53068</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2232,7 +2232,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9557265" y="1990725"/>
-          <a:ext cx="3287877" cy="2484664"/>
+          <a:ext cx="3287877" cy="3586843"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2262,14 +2262,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>372444</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>93889</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>99333</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2287,8 +2287,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9557265" y="4475389"/>
-          <a:ext cx="3287877" cy="2468336"/>
+          <a:off x="9557265" y="5577568"/>
+          <a:ext cx="3287877" cy="3856265"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2318,14 +2318,14 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>110506</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>44903</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>93889</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53068</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2343,8 +2343,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="15960106" y="4467225"/>
-          <a:ext cx="2023094" cy="8164"/>
+          <a:off x="16030863" y="5569403"/>
+          <a:ext cx="2031258" cy="8165"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2374,14 +2374,14 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>102053</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>178253</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2396,8 +2396,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17983200" y="3571875"/>
-          <a:ext cx="1790700" cy="1790700"/>
+          <a:off x="18062121" y="4674053"/>
+          <a:ext cx="1798865" cy="1790700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2432,6 +2432,194 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>258536</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>429986</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>13608</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="77" name="Group 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BC3442-19F3-44E1-8E44-2F9956292463}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5107627" y="4008358"/>
+          <a:ext cx="777586" cy="3053750"/>
+          <a:chOff x="4868636" y="4008358"/>
+          <a:chExt cx="781050" cy="3053750"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="72" name="Oval 71">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C40B20C-6537-40E8-A0B7-7BB1519AB821}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4879521" y="4008358"/>
+            <a:ext cx="753836" cy="756864"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="75" name="Oval 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B6C23B-8DA1-45B9-A982-409582B7E258}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4868636" y="5140472"/>
+            <a:ext cx="753836" cy="756864"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="76" name="Oval 75">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9677758A-C71D-4C9D-A612-FEA9736DA35D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4895850" y="6305244"/>
+            <a:ext cx="753836" cy="756864"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5016,8 +5204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E59531-0B66-425B-ACD4-E8D6EFFE2FF5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD39" sqref="AD39"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
system_overview.xlsx Dataset collection process update2.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63028A40-32F5-4BEF-9FE3-A2B6FDC9AE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB1F5E-E61C-4C37-AAA5-60A337DEE31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="4" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -1287,23 +1287,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>398318</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161055</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>58882</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>174663</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="38" name="Group 37">
+        <xdr:cNvPr id="78" name="Group 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F4DAE9-1B2C-4DA1-B14B-065CBD7E081E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2BCB4D1-99A7-4F3B-B56C-5BD357F333F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1311,18 +1311,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1212273" y="114300"/>
-          <a:ext cx="8647834" cy="3666255"/>
-          <a:chOff x="1771650" y="209550"/>
-          <a:chExt cx="8696325" cy="3666255"/>
+          <a:off x="3429000" y="495300"/>
+          <a:ext cx="18450791" cy="11109363"/>
+          <a:chOff x="1212273" y="114300"/>
+          <a:chExt cx="18450791" cy="11109363"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="27" name="Group 26">
+          <xdr:cNvPr id="38" name="Group 37">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B439411-B979-418A-B830-BE9D3BA034E4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F4DAE9-1B2C-4DA1-B14B-065CBD7E081E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1330,18 +1330,1062 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="1771650" y="209550"/>
-            <a:ext cx="8696325" cy="3666255"/>
-            <a:chOff x="1200150" y="180975"/>
+            <a:off x="1212273" y="114300"/>
+            <a:ext cx="8647834" cy="3666255"/>
+            <a:chOff x="1771650" y="209550"/>
             <a:chExt cx="8696325" cy="3666255"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="27" name="Group 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B439411-B979-418A-B830-BE9D3BA034E4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="1771650" y="209550"/>
+              <a:ext cx="8696325" cy="3666255"/>
+              <a:chOff x="1200150" y="180975"/>
+              <a:chExt cx="8696325" cy="3666255"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="19" name="Rectangle 18">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167517AA-39AE-4E55-B832-CC4AD2954428}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1200150" y="180975"/>
+                <a:ext cx="8696325" cy="3666255"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3458EFC9-8D34-4F48-A8B1-E41072404D3C}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1704975" y="409575"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Simulation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data (MainSimulation.py - CNN)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F299CB2D-04D0-4ABE-BA0B-B0FD6E06795F}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1762125" y="2171700"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>YOLOv3</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF38FEE7-4ABB-463A-A7A6-9DD38C5ACFA3}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="6324600" y="1333500"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Unified</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>(UnifyDataset.py - YOLOv3)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A623ED44-6D0B-43C4-B99F-A2C5230B5890}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="2" idx="3"/>
+                <a:endCxn id="4" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="4876800" y="1133475"/>
+                <a:ext cx="1447800" cy="923925"/>
+              </a:xfrm>
+              <a:prstGeom prst="straightConnector1">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln w="57150">
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="3">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="2">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4495A020-B29D-4DB8-BD65-0BD5497E2A28}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="3" idx="3"/>
+                <a:endCxn id="4" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm flipV="1">
+                <a:off x="4933950" y="2057400"/>
+                <a:ext cx="1390650" cy="838200"/>
+              </a:xfrm>
+              <a:prstGeom prst="straightConnector1">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln w="57150">
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="3">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="2">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+        </xdr:grpSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="35" name="TextBox 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDBA831F-AFBD-4C4A-BC19-608B08FB727A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6953250" y="333375"/>
+              <a:ext cx="3343275" cy="390525"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="57150" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="1"/>
+                <a:t>Dataset collection iteration</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                <a:t> 1</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1400" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="39" name="Group 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FB9299-223C-433D-8C2E-05123C9240E6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1212273" y="7557408"/>
+            <a:ext cx="8647834" cy="3666255"/>
+            <a:chOff x="1771650" y="209550"/>
+            <a:chExt cx="8696325" cy="3666255"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="40" name="Group 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF69B6F-8088-48A5-9544-7ACE4039F940}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="1771650" y="209550"/>
+              <a:ext cx="8696325" cy="3666255"/>
+              <a:chOff x="1200150" y="180975"/>
+              <a:chExt cx="8696325" cy="3666255"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="42" name="Rectangle 41">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBDAA40F-51C2-4E85-8DD8-90CC88835DD6}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1200150" y="180975"/>
+                <a:ext cx="8696325" cy="3666255"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315940E0-4DE3-4817-BD25-1E7774B0FDFB}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1704975" y="409575"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Simulation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data (MainSimulation.py - CNN)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="44" name="Rectangle: Rounded Corners 43">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D1D8C9-4928-4C24-9014-CDE447855DF4}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1762125" y="2171700"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>YOLOv3</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="45" name="Rectangle: Rounded Corners 44">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1897B4CE-C2E4-4F30-BF39-DA0CCE1584E1}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="6324600" y="1333500"/>
+                <a:ext cx="3171825" cy="1447800"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Unified</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> data</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>(UnifyDataset.py - YOLOv3)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4212E485-8854-4681-A0B9-E18314AA348D}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="43" idx="3"/>
+                <a:endCxn id="45" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="4876800" y="1133475"/>
+                <a:ext cx="1447800" cy="923925"/>
+              </a:xfrm>
+              <a:prstGeom prst="straightConnector1">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln w="57150">
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="3">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="2">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F577F37-C557-4212-A3CC-F87973D3A48C}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="44" idx="3"/>
+                <a:endCxn id="45" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm flipV="1">
+                <a:off x="4933950" y="2057400"/>
+                <a:ext cx="1390650" cy="838200"/>
+              </a:xfrm>
+              <a:prstGeom prst="straightConnector1">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln w="57150">
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="3">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="2">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+        </xdr:grpSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="41" name="TextBox 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E18763B-4485-4DF1-B23B-827D44DB2401}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6953250" y="333375"/>
+              <a:ext cx="3343275" cy="390525"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="57150" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="1"/>
+                <a:t>Dataset collection iteration</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                <a:t> n</a:t>
+              </a:r>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1400" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="50" name="Rectangle: Rounded Corners 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A70677-BE10-46AE-8E1B-0691DABC1FC0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12721440" y="3878036"/>
+            <a:ext cx="3148611" cy="3399064"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Combine</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> datasets</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t>(CombineDataset.py - YOLOv3)</a:t>
+            </a:r>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27DE1C-E6CC-4607-9C1D-DD5B646B7362}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="3"/>
+            <a:endCxn id="50" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9464489" y="1990725"/>
+            <a:ext cx="3256951" cy="3586843"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="57150">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1438C6-9E09-4C18-8732-CDAC98FB0E7D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="45" idx="3"/>
+            <a:endCxn id="50" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="9464489" y="5577568"/>
+            <a:ext cx="3256951" cy="3856265"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="57150">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1275AB8-ACE2-4776-867D-DC3EE92A1925}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="50" idx="3"/>
+            <a:endCxn id="66" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="15870051" y="5569403"/>
+            <a:ext cx="2012704" cy="8165"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="57150">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="66" name="Rectangle: Rounded Corners 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD7E897-6210-4864-B6B9-8F42392AAEAD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="17882755" y="4674053"/>
+            <a:ext cx="1780309" cy="1790700"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FinalDataset.csv</a:t>
+            </a:r>
+            <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="77" name="Group 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BC3442-19F3-44E1-8E44-2F9956292463}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5107627" y="4008358"/>
+            <a:ext cx="777586" cy="3053750"/>
+            <a:chOff x="4868636" y="4008358"/>
+            <a:chExt cx="781050" cy="3053750"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="Rectangle 18">
+            <xdr:cNvPr id="72" name="Oval 71">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167517AA-39AE-4E55-B832-CC4AD2954428}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C40B20C-6537-40E8-A0B7-7BB1519AB821}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1349,10 +2393,10 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1200150" y="180975"/>
-              <a:ext cx="8696325" cy="3666255"/>
+              <a:off x="4879521" y="4008358"/>
+              <a:ext cx="753836" cy="756864"/>
             </a:xfrm>
-            <a:prstGeom prst="rect">
+            <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
             <a:solidFill>
@@ -1389,10 +2433,10 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+            <xdr:cNvPr id="75" name="Oval 74">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3458EFC9-8D34-4F48-A8B1-E41072404D3C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B6C23B-8DA1-45B9-A982-409582B7E258}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1400,380 +2444,10 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1704975" y="409575"/>
-              <a:ext cx="3171825" cy="1447800"/>
+              <a:off x="4868636" y="5140472"/>
+              <a:ext cx="753836" cy="756864"/>
             </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>Simulation</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data (MainSimulation.py - CNN)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F299CB2D-04D0-4ABE-BA0B-B0FD6E06795F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1762125" y="2171700"/>
-              <a:ext cx="3171825" cy="1447800"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>YOLOv3</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF38FEE7-4ABB-463A-A7A6-9DD38C5ACFA3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6324600" y="1333500"/>
-              <a:ext cx="3171825" cy="1447800"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>Unified</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t>(UnifyDataset.py - YOLOv3)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A623ED44-6D0B-43C4-B99F-A2C5230B5890}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr>
-              <a:stCxn id="2" idx="3"/>
-              <a:endCxn id="4" idx="1"/>
-            </xdr:cNvCxnSpPr>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4876800" y="1133475"/>
-              <a:ext cx="1447800" cy="923925"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="57150">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="3">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="2">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4495A020-B29D-4DB8-BD65-0BD5497E2A28}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr>
-              <a:stCxn id="3" idx="3"/>
-              <a:endCxn id="4" idx="1"/>
-            </xdr:cNvCxnSpPr>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm flipV="1">
-              <a:off x="4933950" y="2057400"/>
-              <a:ext cx="1390650" cy="838200"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="57150">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="3">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="2">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="TextBox 34">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDBA831F-AFBD-4C4A-BC19-608B08FB727A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6953250" y="333375"/>
-            <a:ext cx="3343275" cy="390525"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="57150" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1"/>
-              <a:t>Dataset collection iteration</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-              <a:t> 1</a:t>
-            </a:r>
-            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>127908</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>174663</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="39" name="Group 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FB9299-223C-433D-8C2E-05123C9240E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1212273" y="7557408"/>
-          <a:ext cx="8647834" cy="3666255"/>
-          <a:chOff x="1771650" y="209550"/>
-          <a:chExt cx="8696325" cy="3666255"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="40" name="Group 39">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF69B6F-8088-48A5-9544-7ACE4039F940}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="1771650" y="209550"/>
-            <a:ext cx="8696325" cy="3666255"/>
-            <a:chOff x="1200150" y="180975"/>
-            <a:chExt cx="8696325" cy="3666255"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="42" name="Rectangle 41">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBDAA40F-51C2-4E85-8DD8-90CC88835DD6}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1200150" y="180975"/>
-              <a:ext cx="8696325" cy="3666255"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
+            <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
             <a:solidFill>
@@ -1810,10 +2484,10 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
+            <xdr:cNvPr id="76" name="Oval 75">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315940E0-4DE3-4817-BD25-1E7774B0FDFB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9677758A-C71D-4C9D-A612-FEA9736DA35D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1821,12 +2495,18 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1704975" y="409575"/>
-              <a:ext cx="3171825" cy="1447800"/>
+              <a:off x="4895850" y="6305244"/>
+              <a:ext cx="753836" cy="756864"/>
             </a:xfrm>
-            <a:prstGeom prst="roundRect">
+            <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </xdr:spPr>
           <xdr:style>
             <a:lnRef idx="2">
@@ -1845,780 +2525,15 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>Simulation</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data (MainSimulation.py - CNN)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="44" name="Rectangle: Rounded Corners 43">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D1D8C9-4928-4C24-9014-CDE447855DF4}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1762125" y="2171700"/>
-              <a:ext cx="3171825" cy="1447800"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>YOLOv3</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t>(PredictYOLOv3.py - YOLOv3)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="45" name="Rectangle: Rounded Corners 44">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1897B4CE-C2E4-4F30-BF39-DA0CCE1584E1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6324600" y="1333500"/>
-              <a:ext cx="3171825" cy="1447800"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600"/>
-                <a:t>Unified</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t> data</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                <a:t>(UnifyDataset.py - YOLOv3)</a:t>
-              </a:r>
-              <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4212E485-8854-4681-A0B9-E18314AA348D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr>
-              <a:stCxn id="43" idx="3"/>
-              <a:endCxn id="45" idx="1"/>
-            </xdr:cNvCxnSpPr>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4876800" y="1133475"/>
-              <a:ext cx="1447800" cy="923925"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="57150">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="3">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="2">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F577F37-C557-4212-A3CC-F87973D3A48C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr>
-              <a:stCxn id="44" idx="3"/>
-              <a:endCxn id="45" idx="1"/>
-            </xdr:cNvCxnSpPr>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm flipV="1">
-              <a:off x="4933950" y="2057400"/>
-              <a:ext cx="1390650" cy="838200"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="57150">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="3">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="2">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
       </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="41" name="TextBox 40">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E18763B-4485-4DF1-B23B-827D44DB2401}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6953250" y="333375"/>
-            <a:ext cx="3343275" cy="390525"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="57150" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1"/>
-              <a:t>Dataset collection iteration</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-              <a:t> n</a:t>
-            </a:r>
-            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>110506</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rectangle: Rounded Corners 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A70677-BE10-46AE-8E1B-0691DABC1FC0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12845142" y="3878036"/>
-          <a:ext cx="3185721" cy="3399064"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600"/>
-            <a:t>Combine</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t> datasets</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>(CombineDataset.py - YOLOv3)</a:t>
-          </a:r>
-          <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>372444</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>53068</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27DE1C-E6CC-4607-9C1D-DD5B646B7362}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="3"/>
-          <a:endCxn id="50" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9557265" y="1990725"/>
-          <a:ext cx="3287877" cy="3586843"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="57150">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>372444</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>53068</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>99333</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1438C6-9E09-4C18-8732-CDAC98FB0E7D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="45" idx="3"/>
-          <a:endCxn id="50" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9557265" y="5577568"/>
-          <a:ext cx="3287877" cy="3856265"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="57150">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>110506</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>44903</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>53068</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1275AB8-ACE2-4776-867D-DC3EE92A1925}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="50" idx="3"/>
-          <a:endCxn id="66" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="16030863" y="5569403"/>
-          <a:ext cx="2031258" cy="8165"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="57150">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>178253</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="66" name="Rectangle: Rounded Corners 65">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD7E897-6210-4864-B6B9-8F42392AAEAD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18062121" y="4674053"/>
-          <a:ext cx="1798865" cy="1790700"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600"/>
-            <a:t>FinalDataset.csv</a:t>
-          </a:r>
-          <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>258536</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>7858</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>429986</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="77" name="Group 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BC3442-19F3-44E1-8E44-2F9956292463}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5107627" y="4008358"/>
-          <a:ext cx="777586" cy="3053750"/>
-          <a:chOff x="4868636" y="4008358"/>
-          <a:chExt cx="781050" cy="3053750"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="72" name="Oval 71">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C40B20C-6537-40E8-A0B7-7BB1519AB821}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4879521" y="4008358"/>
-            <a:ext cx="753836" cy="756864"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="75" name="Oval 74">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B6C23B-8DA1-45B9-A982-409582B7E258}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4868636" y="5140472"/>
-            <a:ext cx="753836" cy="756864"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="76" name="Oval 75">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9677758A-C71D-4C9D-A612-FEA9736DA35D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4895850" y="6305244"/>
-            <a:ext cx="753836" cy="756864"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="sr-Cyrl-RS" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -2924,8 +2839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,10 +3537,10 @@
       <c r="L23" s="43"/>
       <c r="M23" s="43"/>
       <c r="N23" s="44"/>
-      <c r="O23" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P23" s="40"/>
+      <c r="O23" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" s="48"/>
       <c r="Q23" s="35" t="s">
         <v>103</v>
       </c>
@@ -3684,10 +3599,10 @@
       <c r="L25" s="37"/>
       <c r="M25" s="37"/>
       <c r="N25" s="38"/>
-      <c r="O25" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P25" s="40"/>
+      <c r="O25" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="48"/>
       <c r="Q25" s="34" t="s">
         <v>136</v>
       </c>
@@ -5205,7 +5120,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+      <selection activeCell="AP27" sqref="AP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PredictYOLOv3.py modified to consider only objects of interest in datasets.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB1F5E-E61C-4C37-AAA5-60A337DEE31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BF85A7-04BD-4E72-9768-B7127DF15A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="4" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="141">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -413,9 +413,6 @@
     <t>The system shall come with fully functionl configuration scripts for generating CARLA simulator scenarios in form of python scripts.</t>
   </si>
   <si>
-    <t>./util/*</t>
-  </si>
-  <si>
     <t>The system shall be able to aquire all relevant information from the CARLA simulator scenarios needed for the training of the CNN neural network.</t>
   </si>
   <si>
@@ -823,6 +820,22 @@
   </si>
   <si>
     <t>./cnn/CNNPredict.py</t>
+  </si>
+  <si>
+    <t>./util/Config.py
+./util/GenerateTraffic.py</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting in form of python script.</t>
+  </si>
+  <si>
+    <t>./util/CombineDatasets.py</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2196,7 @@
             <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t>(CombineDataset.py - YOLOv3)</a:t>
+              <a:t>(CombineDatasets.py - YOLOv3)</a:t>
             </a:r>
             <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
           </a:p>
@@ -2837,10 +2850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25:P25"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,7 +2989,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
@@ -3025,7 +3038,7 @@
       </c>
       <c r="P6" s="46"/>
       <c r="Q6" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R6" s="34"/>
       <c r="S6" s="34"/>
@@ -3085,7 +3098,7 @@
       </c>
       <c r="P8" s="46"/>
       <c r="Q8" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
@@ -3201,7 +3214,7 @@
       <c r="M12" s="37"/>
       <c r="N12" s="38"/>
       <c r="O12" s="39" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="P12" s="40"/>
       <c r="Q12" s="49" t="s">
@@ -3356,7 +3369,7 @@
       </c>
       <c r="P17" s="48"/>
       <c r="Q17" s="35" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="R17" s="35"/>
       <c r="S17" s="35"/>
@@ -3366,10 +3379,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="36" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>67</v>
       </c>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
@@ -3387,7 +3400,7 @@
       </c>
       <c r="P18" s="48"/>
       <c r="Q18" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
@@ -3397,10 +3410,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>69</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>70</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
@@ -3418,7 +3431,7 @@
       </c>
       <c r="P19" s="46"/>
       <c r="Q19" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R19" s="35"/>
       <c r="S19" s="35"/>
@@ -3428,10 +3441,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="36" t="s">
         <v>71</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>72</v>
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -3449,7 +3462,7 @@
       </c>
       <c r="P20" s="46"/>
       <c r="Q20" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R20" s="34"/>
       <c r="S20" s="34"/>
@@ -3459,10 +3472,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
@@ -3480,7 +3493,7 @@
       </c>
       <c r="P21" s="46"/>
       <c r="Q21" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R21" s="35"/>
       <c r="S21" s="35"/>
@@ -3490,10 +3503,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>81</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
@@ -3511,7 +3524,7 @@
       </c>
       <c r="P22" s="48"/>
       <c r="Q22" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R22" s="34"/>
       <c r="S22" s="34"/>
@@ -3521,10 +3534,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>100</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>101</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
@@ -3542,7 +3555,7 @@
       </c>
       <c r="P23" s="48"/>
       <c r="Q23" s="35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R23" s="35"/>
       <c r="S23" s="35"/>
@@ -3552,10 +3565,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>104</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>105</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
@@ -3569,11 +3582,11 @@
       <c r="M24" s="37"/>
       <c r="N24" s="38"/>
       <c r="O24" s="39" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="P24" s="40"/>
       <c r="Q24" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R24" s="34"/>
       <c r="S24" s="34"/>
@@ -3583,10 +3596,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>134</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>135</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -3604,13 +3617,47 @@
       </c>
       <c r="P25" s="48"/>
       <c r="Q25" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R25" s="34"/>
       <c r="S25" s="34"/>
     </row>
+    <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="76">
+    <mergeCell ref="C26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:S26"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="Q14:S14"/>
@@ -3734,7 +3781,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
@@ -3768,7 +3815,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -3782,7 +3829,7 @@
       <c r="H3" s="64"/>
       <c r="I3" s="64"/>
       <c r="J3" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="69"/>
       <c r="L3" s="69"/>
@@ -3790,7 +3837,7 @@
       <c r="N3" s="69"/>
       <c r="O3" s="69"/>
       <c r="P3" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="67"/>
       <c r="R3" s="67"/>
@@ -3802,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -3836,7 +3883,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
@@ -3870,7 +3917,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -3904,7 +3951,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -3938,13 +3985,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>73</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>74</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
@@ -3952,7 +3999,7 @@
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
       <c r="J8" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K8" s="51"/>
       <c r="L8" s="51"/>
@@ -3972,13 +4019,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="58"/>
@@ -3986,7 +4033,7 @@
       <c r="H9" s="58"/>
       <c r="I9" s="59"/>
       <c r="J9" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K9" s="61"/>
       <c r="L9" s="61"/>
@@ -3994,7 +4041,7 @@
       <c r="N9" s="61"/>
       <c r="O9" s="62"/>
       <c r="P9" s="66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="66"/>
       <c r="R9" s="66"/>
@@ -4006,13 +4053,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
@@ -4020,7 +4067,7 @@
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
       <c r="J10" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="51"/>
@@ -4028,7 +4075,7 @@
       <c r="N10" s="51"/>
       <c r="O10" s="52"/>
       <c r="P10" s="65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="65"/>
       <c r="R10" s="65"/>
@@ -4163,7 +4210,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -4206,10 +4253,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>118</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>119</v>
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
@@ -4227,10 +4274,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
@@ -4248,10 +4295,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="60" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>122</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
@@ -4269,7 +4316,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="50">
         <v>0.25</v>
@@ -4290,10 +4337,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="61"/>
       <c r="E7" s="61"/>
@@ -4311,10 +4358,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>122</v>
       </c>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
@@ -4332,7 +4379,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="60">
         <v>0.25</v>
@@ -4353,10 +4400,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
@@ -4374,10 +4421,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="60" t="s">
         <v>121</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>122</v>
       </c>
       <c r="D11" s="61"/>
       <c r="E11" s="61"/>
@@ -4395,7 +4442,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="50">
         <v>0.25</v>
@@ -4416,7 +4463,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="60"/>
       <c r="D13" s="61"/>
@@ -4435,10 +4482,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="51"/>
       <c r="E14" s="51"/>
@@ -4456,7 +4503,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="60">
         <v>0.25</v>
@@ -4477,10 +4524,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
@@ -4498,7 +4545,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="60">
         <v>0.25</v>
@@ -4519,10 +4566,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="51"/>
@@ -4540,10 +4587,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19" s="61"/>
       <c r="E19" s="61"/>
@@ -4551,7 +4598,7 @@
       <c r="G19" s="61"/>
       <c r="H19" s="62"/>
       <c r="I19" s="66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J19" s="66"/>
       <c r="K19" s="66"/>
@@ -4620,7 +4667,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -4644,35 +4691,35 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="74" t="s">
         <v>89</v>
-      </c>
-      <c r="C2" s="74" t="s">
-        <v>90</v>
       </c>
       <c r="D2" s="76"/>
       <c r="E2" s="74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="75"/>
       <c r="G2" s="75"/>
       <c r="H2" s="76"/>
       <c r="I2" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="53"/>
       <c r="K2" s="53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L2" s="82"/>
       <c r="M2" s="74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N2" s="84"/>
       <c r="O2" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P2" s="74" t="s">
         <v>4</v>
@@ -4699,28 +4746,28 @@
       </c>
       <c r="D3" s="79"/>
       <c r="E3" s="77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="80"/>
       <c r="G3" s="80"/>
       <c r="H3" s="81"/>
       <c r="I3" s="77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" s="79"/>
       <c r="K3" s="83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="81"/>
       <c r="M3" s="83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="81"/>
       <c r="O3" s="27" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="78"/>
       <c r="R3" s="78"/>
@@ -5120,7 +5167,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AP27" sqref="AP27"/>
+      <selection activeCell="Z43" sqref="Z43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Placeholder for CombineDatasets.py added. Removed unnecessary imports from other files.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BF85A7-04BD-4E72-9768-B7127DF15A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E4C55E-2E8A-4EE6-926F-A458DB306019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="4" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -810,9 +810,6 @@
     <t>output_no</t>
   </si>
   <si>
-    <t>To be finaly determined.</t>
-  </si>
-  <si>
     <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation</t>
   </si>
   <si>
@@ -836,6 +833,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>To be finally determined.</t>
   </si>
 </sst>
 </file>
@@ -2853,7 +2853,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="O17" sqref="O17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,7 +3214,7 @@
       <c r="M12" s="37"/>
       <c r="N12" s="38"/>
       <c r="O12" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P12" s="40"/>
       <c r="Q12" s="49" t="s">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="P17" s="48"/>
       <c r="Q17" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R17" s="35"/>
       <c r="S17" s="35"/>
@@ -3582,7 +3582,7 @@
       <c r="M24" s="37"/>
       <c r="N24" s="38"/>
       <c r="O24" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P24" s="40"/>
       <c r="Q24" s="41" t="s">
@@ -3596,10 +3596,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>133</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>134</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="P25" s="48"/>
       <c r="Q25" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R25" s="34"/>
       <c r="S25" s="34"/>
@@ -3627,10 +3627,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="36" t="s">
         <v>137</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>138</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
@@ -3644,11 +3644,11 @@
       <c r="M26" s="37"/>
       <c r="N26" s="38"/>
       <c r="O26" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P26" s="40"/>
       <c r="Q26" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R26" s="34"/>
       <c r="S26" s="34"/>
@@ -4199,8 +4199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3399D5AB-0FA1-4FE2-AE54-B718FE78F3AD}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4598,7 +4598,7 @@
       <c r="G19" s="61"/>
       <c r="H19" s="62"/>
       <c r="I19" s="66" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J19" s="66"/>
       <c r="K19" s="66"/>
@@ -4655,7 +4655,7 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:T3"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5166,7 +5166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E59531-0B66-425B-ACD4-E8D6EFFE2FF5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Z43" sqref="Z43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIne tunning hyper-parameters, model optimizer changed from ADAM to SGD, loss function to binary crossentropy.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD238D5-D127-402A-85A8-D30796F675CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB67904-02B3-4DC2-8A8B-4E97E7A759BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="1" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -754,11 +754,6 @@
     </r>
   </si>
   <si>
-    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't
-RoI = 1280 - 0 x 720 - 350 = 1280 x 370 
-Upper 350 pixels in all directions can be removed from the image. Image can be cropped to 1280x370</t>
-  </si>
-  <si>
     <t>CNN Architecture</t>
   </si>
   <si>
@@ -866,6 +861,24 @@
       </rPr>
       <t>: Accuracies not avaliable, from memory: Training 0.6, Validation 0.7, Test validation 0.65</t>
     </r>
+  </si>
+  <si>
+    <t>Active supervised</t>
+  </si>
+  <si>
+    <t>Contains images from town01, town02 and town06 from previous iteration (town06 labeled).
+Active supervised learning with 2163 unique inaccurate labels detected.
+Vpresent = 473
+Vpl = 467
+Vpr = 427
+Vpc = 425
+safeToAcc = 371
+Total inaccurate = 2163 (Total labels = (2321 - 1218) * 5 = 5515)</t>
+  </si>
+  <si>
+    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't
+RoI = 1280 - 0 x 720 - 350 = 1280 x 370 
+Upper 350 pixels in all directions can be removed from the image. Image can be cropped to 1280x370</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1137,9 +1150,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1166,21 +1176,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1205,12 +1227,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1223,18 +1239,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1318,6 +1334,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,7 +1381,7 @@
         <xdr:cNvPr id="78" name="Group 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2BCB4D1-99A7-4F3B-B56C-5BD357F333F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1375,7 +1400,7 @@
           <xdr:cNvPr id="38" name="Group 37">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F4DAE9-1B2C-4DA1-B14B-065CBD7E081E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1394,7 +1419,7 @@
             <xdr:cNvPr id="27" name="Group 26">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B439411-B979-418A-B830-BE9D3BA034E4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1413,7 +1438,7 @@
               <xdr:cNvPr id="19" name="Rectangle 18">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167517AA-39AE-4E55-B832-CC4AD2954428}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1464,7 +1489,7 @@
               <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3458EFC9-8D34-4F48-A8B1-E41072404D3C}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1517,7 +1542,7 @@
               <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F299CB2D-04D0-4ABE-BA0B-B0FD6E06795F}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1577,7 +1602,7 @@
               <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF38FEE7-4ABB-463A-A7A6-9DD38C5ACFA3}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1637,7 +1662,7 @@
               <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A623ED44-6D0B-43C4-B99F-A2C5230B5890}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1678,7 +1703,7 @@
               <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4495A020-B29D-4DB8-BD65-0BD5497E2A28}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1720,7 +1745,7 @@
             <xdr:cNvPr id="35" name="TextBox 34">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDBA831F-AFBD-4C4A-BC19-608B08FB727A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1781,7 +1806,7 @@
           <xdr:cNvPr id="39" name="Group 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FB9299-223C-433D-8C2E-05123C9240E6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1800,7 +1825,7 @@
             <xdr:cNvPr id="40" name="Group 39">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF69B6F-8088-48A5-9544-7ACE4039F940}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1819,7 +1844,7 @@
               <xdr:cNvPr id="42" name="Rectangle 41">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBDAA40F-51C2-4E85-8DD8-90CC88835DD6}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1870,7 +1895,7 @@
               <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{315940E0-4DE3-4817-BD25-1E7774B0FDFB}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1923,7 +1948,7 @@
               <xdr:cNvPr id="44" name="Rectangle: Rounded Corners 43">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D1D8C9-4928-4C24-9014-CDE447855DF4}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002C000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1983,7 +2008,7 @@
               <xdr:cNvPr id="45" name="Rectangle: Rounded Corners 44">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1897B4CE-C2E4-4F30-BF39-DA0CCE1584E1}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2043,7 +2068,7 @@
               <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4212E485-8854-4681-A0B9-E18314AA348D}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2084,7 +2109,7 @@
               <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F577F37-C557-4212-A3CC-F87973D3A48C}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F000000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -2126,7 +2151,7 @@
             <xdr:cNvPr id="41" name="TextBox 40">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E18763B-4485-4DF1-B23B-827D44DB2401}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2187,7 +2212,7 @@
           <xdr:cNvPr id="50" name="Rectangle: Rounded Corners 49">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A70677-BE10-46AE-8E1B-0691DABC1FC0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2236,7 +2261,7 @@
             <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t>(CombineDatasets.py - YOLOv3)</a:t>
+              <a:t>(CombineDatasets.py)</a:t>
             </a:r>
             <a:endParaRPr lang="sr-Cyrl-RS" sz="1600"/>
           </a:p>
@@ -2247,7 +2272,7 @@
           <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27DE1C-E6CC-4607-9C1D-DD5B646B7362}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2288,7 +2313,7 @@
           <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1438C6-9E09-4C18-8732-CDAC98FB0E7D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2329,7 +2354,7 @@
           <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1275AB8-ACE2-4776-867D-DC3EE92A1925}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2370,7 +2395,7 @@
           <xdr:cNvPr id="66" name="Rectangle: Rounded Corners 65">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD7E897-6210-4864-B6B9-8F42392AAEAD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2419,7 +2444,7 @@
           <xdr:cNvPr id="77" name="Group 76">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BC3442-19F3-44E1-8E44-2F9956292463}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2427,10 +2452,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="5107627" y="4008358"/>
-            <a:ext cx="777586" cy="3053750"/>
+            <a:off x="5107623" y="4008358"/>
+            <a:ext cx="750530" cy="3053750"/>
             <a:chOff x="4868636" y="4008358"/>
-            <a:chExt cx="781050" cy="3053750"/>
+            <a:chExt cx="753874" cy="3053750"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -2438,7 +2463,7 @@
             <xdr:cNvPr id="72" name="Oval 71">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C40B20C-6537-40E8-A0B7-7BB1519AB821}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000048000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2446,7 +2471,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4879521" y="4008358"/>
+              <a:off x="4868650" y="4008358"/>
               <a:ext cx="753836" cy="756864"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
@@ -2489,7 +2514,7 @@
             <xdr:cNvPr id="75" name="Oval 74">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B6C23B-8DA1-45B9-A982-409582B7E258}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2540,7 +2565,7 @@
             <xdr:cNvPr id="76" name="Oval 75">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9677758A-C71D-4C9D-A612-FEA9736DA35D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2548,7 +2573,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4895850" y="6305244"/>
+              <a:off x="4868674" y="6305244"/>
               <a:ext cx="753836" cy="756864"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
@@ -2588,6 +2613,483 @@
         </xdr:sp>
       </xdr:grpSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>22241</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>22242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11089821" y="1741715"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>370115</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>70758</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>324320</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>65785</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6493329" y="832758"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>427265</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>100693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381470</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6550479" y="2577193"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>335205</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76669</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6504214" y="8273142"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>451757</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>111577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>405962</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>106604</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6574971" y="10017577"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>46262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>68505</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>41289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11136085" y="9190262"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>267171</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>103885</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36" descr="Text x python Icon | Leaf Mimes Iconset | Untergunter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17457965" y="4490358"/>
+          <a:ext cx="566527" cy="566527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>75645</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>12193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>108774</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20752222" y="6108193"/>
+          <a:ext cx="641264" cy="646043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2892,8 +3394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,27 +3408,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2938,26 +3440,26 @@
       <c r="C2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
       <c r="O2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="59"/>
+      <c r="P2" s="60"/>
       <c r="Q2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="60"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -2966,29 +3468,29 @@
       <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="51" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="39" t="s">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -2997,29 +3499,29 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="49" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="38" t="s">
+      <c r="P4" s="53"/>
+      <c r="Q4" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -3028,29 +3530,29 @@
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="49" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="39" t="s">
+      <c r="P5" s="53"/>
+      <c r="Q5" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -3059,29 +3561,29 @@
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="49" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="38" t="s">
+      <c r="P6" s="53"/>
+      <c r="Q6" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -3090,27 +3592,27 @@
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="51" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -3119,29 +3621,29 @@
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="49" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="38" t="s">
+      <c r="P8" s="53"/>
+      <c r="Q8" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -3150,27 +3652,27 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="51" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -3179,29 +3681,29 @@
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="49" t="s">
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="38" t="s">
+      <c r="P10" s="53"/>
+      <c r="Q10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -3210,27 +3712,27 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="51" t="s">
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -3239,29 +3741,29 @@
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="53" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -3270,27 +3772,27 @@
       <c r="B13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="49" t="s">
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -3299,27 +3801,27 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="51" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -3328,29 +3830,29 @@
       <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="51" t="s">
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="39" t="s">
+      <c r="P15" s="43"/>
+      <c r="Q15" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -3359,29 +3861,29 @@
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="51" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="38" t="s">
+      <c r="P16" s="43"/>
+      <c r="Q16" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -3390,29 +3892,29 @@
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="51" t="s">
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -3421,29 +3923,29 @@
       <c r="B18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="51" t="s">
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="38" t="s">
+      <c r="P18" s="43"/>
+      <c r="Q18" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -3452,29 +3954,29 @@
       <c r="B19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="49" t="s">
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="39" t="s">
+      <c r="P19" s="53"/>
+      <c r="Q19" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -3483,29 +3985,29 @@
       <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="49" t="s">
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="38" t="s">
+      <c r="P20" s="53"/>
+      <c r="Q20" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
+      <c r="R20" s="44"/>
+      <c r="S20" s="44"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -3514,29 +4016,29 @@
       <c r="B21" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="49" t="s">
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="39" t="s">
+      <c r="P21" s="53"/>
+      <c r="Q21" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -3545,29 +4047,29 @@
       <c r="B22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="51" t="s">
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="38" t="s">
+      <c r="P22" s="43"/>
+      <c r="Q22" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="44"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -3576,29 +4078,29 @@
       <c r="B23" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="51" t="s">
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="39" t="s">
+      <c r="P23" s="43"/>
+      <c r="Q23" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -3607,91 +4109,91 @@
       <c r="B24" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="P24" s="44"/>
-      <c r="Q24" s="45" t="s">
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
     </row>
     <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>24</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -3781,8 +4283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2E6D2C-5E3C-49D0-A2B0-F322C3268B9A}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,28 +4295,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3826,29 +4328,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="60" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="74" t="s">
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -3860,29 +4362,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="39" t="s">
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="72"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="73"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3894,29 +4396,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="54" t="s">
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="69" t="s">
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3928,29 +4430,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64" t="s">
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="70" t="s">
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -3962,29 +4464,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="54" t="s">
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="69" t="s">
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -3996,29 +4498,29 @@
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64" t="s">
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="70" t="s">
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="70"/>
-      <c r="S7" s="70"/>
-      <c r="T7" s="70"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4030,29 +4532,29 @@
       <c r="C8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="54" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="69" t="s">
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4064,29 +4566,29 @@
       <c r="C9" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="64" t="s">
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="70" t="s">
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -4095,32 +4597,32 @@
       <c r="B10" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="54" t="s">
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="69" t="s">
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -4249,401 +4751,401 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
+      <c r="A1" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="74" t="s">
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="73"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
+      <c r="B4" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="54">
+      <c r="B6" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="55">
         <v>0.25</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
+      <c r="B7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="64">
+      <c r="B9" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="65">
         <v>0.25</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
+      <c r="B10" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="54">
+      <c r="B12" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="55">
         <v>0.25</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="70"/>
+      <c r="B13" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="65"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
+      <c r="B14" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="64">
+      <c r="B15" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="65">
         <v>0.25</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
+      <c r="B16" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="64">
+      <c r="B17" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="65">
         <v>0.25</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
+      <c r="B18" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
+      <c r="B19" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -4695,41 +5197,41 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:U4"/>
+      <selection activeCell="E4" sqref="E4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="34" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" style="33" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4738,41 +5240,41 @@
       <c r="B2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="78" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="57" t="s">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="86"/>
-      <c r="M2" s="78" t="s">
+      <c r="L2" s="87"/>
+      <c r="M2" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="N2" s="88"/>
-      <c r="O2" s="37" t="s">
-        <v>140</v>
+      <c r="N2" s="89"/>
+      <c r="O2" s="36" t="s">
+        <v>139</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="81"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -4786,71 +5288,83 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="81">
+      <c r="C3" s="82">
         <v>5</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="81" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="83"/>
-      <c r="K3" s="87" t="s">
+      <c r="J3" s="84"/>
+      <c r="K3" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="85"/>
-      <c r="M3" s="87" t="s">
+      <c r="L3" s="86"/>
+      <c r="M3" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="N3" s="85"/>
-      <c r="O3" s="33" t="s">
+      <c r="N3" s="86"/>
+      <c r="O3" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="P3" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="81" t="s">
-        <v>142</v>
-      </c>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="82"/>
-      <c r="U3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="84"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="56"/>
+      <c r="B4" s="21">
+        <v>2321</v>
+      </c>
+      <c r="C4" s="55">
+        <v>5</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="P4" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="57"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
@@ -4862,19 +5376,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="36"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="35"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="22"/>
@@ -4892,25 +5406,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="56"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="57"/>
       <c r="O6" s="21"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="56"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="57"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -4922,19 +5436,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="36"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="19"/>
       <c r="R7" s="22"/>
@@ -4952,25 +5466,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="56"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="57"/>
       <c r="O8" s="21"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="56"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="57"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -4982,19 +5496,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="36"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="35"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19"/>
       <c r="R9" s="22"/>
@@ -5012,44 +5526,44 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="56"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="21"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="56"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="57"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="36"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="35"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="22"/>
@@ -5062,25 +5576,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="56"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="57"/>
       <c r="O12" s="21"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="56"/>
+      <c r="Q12" s="55"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="57"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -5146,7 +5660,7 @@
       <c r="U15" s="15"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F16" s="28"/>
+      <c r="F16" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="63">
@@ -5223,8 +5737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E59531-0B66-425B-ACD4-E8D6EFFE2FF5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF58" sqref="AF58"/>
+    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG45" sqref="AG45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes regarding model input size, hyper-parameters, parameters of the model. Adaptation of scripts in respect to mentioned changes. Scripts CropImgs.py and RenameImgs.py added.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB67904-02B3-4DC2-8A8B-4E97E7A759BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3937E506-7096-4AC6-B8A2-480BB75EE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="1" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="146">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -158,65 +158,6 @@
     <t>Vehicle in the same lane</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">0 - Vehicles present on the current image
-1 - Vehicles </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> present on the current image</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0 - Vehicle in the same lane as the driver vehicle
-1 - Vehicle </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in the same lane as the driver vehicle</t>
-    </r>
-  </si>
-  <si>
-    <t>0 - Safe to accelerate (too far from the leading vehicle)
- 0.5 - Accelerate at the same rate (the distance is "just right")
-1 - Not safe to accelerate (too close to the leading vehicle)</t>
-  </si>
-  <si>
     <t>Describes if the detected traffic is in the lane of the driver vehicle. Marks the existance of the leading vehicle.</t>
   </si>
   <si>
@@ -655,6 +596,271 @@
     <t>Describes that there are vehicles in adject right lane relative to the driving lane</t>
   </si>
   <si>
+    <t>ID-2, ID-3, ID-5, ID-7, ID-8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Related to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CNN parameter ID-7, ID-8.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Related to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CNN parameter ID-2, ID-6, ID-7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ID-8</t>
+    </r>
+  </si>
+  <si>
+    <t>CNN Architecture</t>
+  </si>
+  <si>
+    <t>Input layer</t>
+  </si>
+  <si>
+    <t>100x100</t>
+  </si>
+  <si>
+    <t>Conv2D(16, (3,3), activation= 'relu')</t>
+  </si>
+  <si>
+    <t>Max-pooling layer</t>
+  </si>
+  <si>
+    <t>pool_size = (2, 2)</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>Conv2D(32, (3,3), activation= 'relu')</t>
+  </si>
+  <si>
+    <t>Conv2D(64, (3,3), activation='relu')</t>
+  </si>
+  <si>
+    <t>Flatten</t>
+  </si>
+  <si>
+    <t>Dense layer</t>
+  </si>
+  <si>
+    <t>Convolutive layer</t>
+  </si>
+  <si>
+    <t>Dense(32, activation='relu')</t>
+  </si>
+  <si>
+    <t>Dense(64, activation='relu')</t>
+  </si>
+  <si>
+    <t>Dense(128, activation='relu')</t>
+  </si>
+  <si>
+    <t>output_no</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation in form of python script.</t>
+  </si>
+  <si>
+    <t>./cnn/CNNPredict.py</t>
+  </si>
+  <si>
+    <t>./util/Config.py
+./util/GenerateTraffic.py</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting</t>
+  </si>
+  <si>
+    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting in form of python script.</t>
+  </si>
+  <si>
+    <t>./util/CombineDatasets.py</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>To be finally determined.</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Supervised</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimal set of parameters used for determining the successfulness of the CNN to be used in the system.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Accuracies not avaliable, from memory: Training 0.6, Validation 0.7, Test validation 0.65</t>
+    </r>
+  </si>
+  <si>
+    <t>Active supervised</t>
+  </si>
+  <si>
+    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't
+RoI = 1280 - 0 x 720 - 350 = 1280 x 370 
+Upper 350 pixels in all directions can be removed from the image. Image can be cropped to 1280x370</t>
+  </si>
+  <si>
+    <t>Contains images from town01, town02 and town06 from previous iteration (town06 labeled).
+Active supervised learning with 2163 unique inaccurate labels detected.
+Vpresent = 473
+Vpl = 467
+Vpr = 427
+Vpc = 425
+safeToAcc = 371
+Total inaccurate = 2163 (Total labels = (2321 - 1218) * 5 = 5515)
+Model changes:
+optimizer=SGD(lr=0.01, momentum=0.9)
+loss='binary_crossentropy'
+metrics=BinaryAccuracy(name = 'binary_accuracy', threshold = 0.05)
+best results with:
+batchSize=4
+ReduceLROnPlateau(factor=0.0025)
+monitor='val_binary_accuracy'</t>
+  </si>
+  <si>
+    <t>Contains images from town01, town02 and town06, some images were left out from previous iteration (redudancy), as well as some labels were corrected by hand.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 - Vehicles </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> present on the current image
+1 - Vehicles present on the current image</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 - Safe to accelerate (too far from the leading vehicle)
+ 0.5 - Accelerate at the same rate (the distance is "just right")
+1 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> safe to accelerate (too close to the leading vehicle)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 - Vehicle </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the same lane as the driver vehicle
+1 - Vehicle in the same lane as the driver vehicle</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">0 - Vehicles present in adjecent left lane
 1 - Vehicles </t>
@@ -683,7 +889,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1 - Vehicles present in adjecent right lane
+      <t xml:space="preserve">0 - Vehicles present in adjecent right lane
 1 - Vehicles </t>
     </r>
     <r>
@@ -707,178 +913,6 @@
       </rPr>
       <t xml:space="preserve"> present in adjecent right lane</t>
     </r>
-  </si>
-  <si>
-    <t>ID-2, ID-3, ID-5, ID-7, ID-8</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Related to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CNN parameter ID-7, ID-8.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Related to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CNN parameter ID-2, ID-6, ID-7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, ID-8</t>
-    </r>
-  </si>
-  <si>
-    <t>CNN Architecture</t>
-  </si>
-  <si>
-    <t>Input layer</t>
-  </si>
-  <si>
-    <t>100x100</t>
-  </si>
-  <si>
-    <t>Conv2D(16, (3,3), activation= 'relu')</t>
-  </si>
-  <si>
-    <t>Max-pooling layer</t>
-  </si>
-  <si>
-    <t>pool_size = (2, 2)</t>
-  </si>
-  <si>
-    <t>Dropout</t>
-  </si>
-  <si>
-    <t>Conv2D(32, (3,3), activation= 'relu')</t>
-  </si>
-  <si>
-    <t>Conv2D(64, (3,3), activation='relu')</t>
-  </si>
-  <si>
-    <t>Flatten</t>
-  </si>
-  <si>
-    <t>Dense layer</t>
-  </si>
-  <si>
-    <t>Convolutive layer</t>
-  </si>
-  <si>
-    <t>Dense(32, activation='relu')</t>
-  </si>
-  <si>
-    <t>Dense(64, activation='relu')</t>
-  </si>
-  <si>
-    <t>Dense(128, activation='relu')</t>
-  </si>
-  <si>
-    <t>output_no</t>
-  </si>
-  <si>
-    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation</t>
-  </si>
-  <si>
-    <t>The system shall come with fully functional script for CNN predicting isolated from the main simulation in form of python script.</t>
-  </si>
-  <si>
-    <t>./cnn/CNNPredict.py</t>
-  </si>
-  <si>
-    <t>./util/Config.py
-./util/GenerateTraffic.py</t>
-  </si>
-  <si>
-    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting</t>
-  </si>
-  <si>
-    <t>The system shall come with fully functional script for combining datasets from multiple iterations of dataset collecting in form of python script.</t>
-  </si>
-  <si>
-    <t>./util/CombineDatasets.py</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>To be finally determined.</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Supervised</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Minimal set of parameters used for determining the successfulness of the CNN to be used in the system.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Accuracies not avaliable, from memory: Training 0.6, Validation 0.7, Test validation 0.65</t>
-    </r>
-  </si>
-  <si>
-    <t>Active supervised</t>
-  </si>
-  <si>
-    <t>Contains images from town01, town02 and town06 from previous iteration (town06 labeled).
-Active supervised learning with 2163 unique inaccurate labels detected.
-Vpresent = 473
-Vpl = 467
-Vpr = 427
-Vpc = 425
-safeToAcc = 371
-Total inaccurate = 2163 (Total labels = (2321 - 1218) * 5 = 5515)</t>
-  </si>
-  <si>
-    <t>Size is debatable. Do we need whole image for the lane processing? Do we need the sky? - We don't
-RoI = 1280 - 0 x 720 - 350 = 1280 x 370 
-Upper 350 pixels in all directions can be removed from the image. Image can be cropped to 1280x370</t>
   </si>
 </sst>
 </file>
@@ -916,7 +950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,6 +996,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1179,7 +1219,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3408,792 +3454,792 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="58" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="59"/>
-      <c r="S2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="62"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
+      <c r="C4" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
+        <v>28</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
+        <v>31</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
+        <v>35</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
+        <v>40</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
+        <v>46</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
+        <v>50</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
+        <v>52</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="46"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
+      <c r="C16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
+        <v>60</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
+        <v>62</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="R20" s="44"/>
-      <c r="S20" s="44"/>
+        <v>67</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
+        <v>72</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="47"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="R24" s="44"/>
-      <c r="S24" s="44"/>
+        <v>99</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="R25" s="44"/>
-      <c r="S25" s="44"/>
+        <v>125</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
     </row>
     <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>24</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
+        <v>129</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -4284,7 +4330,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4295,334 +4341,334 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="59" t="s">
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="75" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="73"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="75"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="70" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="71" t="s">
+      <c r="D5" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="55" t="s">
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="70" t="s">
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="72"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="71" t="s">
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q9" s="71"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
+        <v>102</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
+        <v>103</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -4751,401 +4797,401 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="75" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="73"/>
+        <v>110</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="75"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
+        <v>120</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
+        <v>113</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="55">
+        <v>115</v>
+      </c>
+      <c r="C6" s="57">
         <v>0.25</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+        <v>120</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
+        <v>113</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="65">
+        <v>115</v>
+      </c>
+      <c r="C9" s="67">
         <v>0.25</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
+        <v>120</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
+        <v>113</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="55">
+        <v>115</v>
+      </c>
+      <c r="C12" s="57">
         <v>0.25</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
+        <v>118</v>
+      </c>
+      <c r="C13" s="67"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="70"/>
+        <v>119</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="65">
+        <v>115</v>
+      </c>
+      <c r="C15" s="67">
         <v>0.25</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
+        <v>119</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="65">
+        <v>115</v>
+      </c>
+      <c r="C17" s="67">
         <v>0.25</v>
       </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
+        <v>119</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
       <c r="B19" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="J19" s="71"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="71"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -5196,8 +5242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:H4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5209,72 +5255,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="79" t="s">
+      <c r="L2" s="89"/>
+      <c r="M2" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="L2" s="87"/>
-      <c r="M2" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="N2" s="89"/>
+      <c r="N2" s="91"/>
       <c r="O2" s="36" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="81"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="83"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -5288,113 +5334,137 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="84">
         <v>5</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="88" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="86"/>
-      <c r="M3" s="88" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="86"/>
+      <c r="K3" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="88"/>
+      <c r="M3" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="88"/>
       <c r="O3" s="32" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P3" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="84"/>
+        <v>23</v>
+      </c>
+      <c r="Q3" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="86"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="21">
         <v>2321</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="57">
         <v>5</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="57"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="57">
+        <v>0.97</v>
+      </c>
+      <c r="J4" s="59"/>
+      <c r="K4" s="57">
+        <v>0.96458999999999995</v>
+      </c>
+      <c r="L4" s="59"/>
+      <c r="M4" s="57">
+        <v>0.94051739999999995</v>
+      </c>
+      <c r="N4" s="59"/>
       <c r="O4" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="P4" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="57"/>
+        <v>137</v>
+      </c>
+      <c r="P4" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="59"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="24"/>
+      <c r="B5" s="23">
+        <v>2048</v>
+      </c>
+      <c r="C5" s="84">
+        <v>5</v>
+      </c>
+      <c r="D5" s="86"/>
+      <c r="E5" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="86"/>
+      <c r="K5" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="88"/>
+      <c r="M5" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="88"/>
+      <c r="O5" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="P5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="86"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
@@ -5406,25 +5476,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="59"/>
       <c r="O6" s="21"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="59"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -5436,18 +5506,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="86"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="88"/>
       <c r="O7" s="35"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="19"/>
@@ -5466,25 +5536,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="59"/>
       <c r="O8" s="21"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="57"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="59"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -5496,18 +5566,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="86"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="88"/>
       <c r="O9" s="35"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19"/>
@@ -5526,43 +5596,43 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="59"/>
       <c r="O10" s="21"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="59"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="86"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="88"/>
       <c r="O11" s="35"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="19"/>
@@ -5576,25 +5646,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="59"/>
       <c r="O12" s="21"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="59"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -5663,7 +5733,7 @@
       <c r="F16" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="64">
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="Q10:U10"/>
@@ -5711,6 +5781,7 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="Q5:U5"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="Q2:U2"/>
@@ -5737,8 +5808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E59531-0B66-425B-ACD4-E8D6EFFE2FF5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG45" sqref="AG45"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
system_overview.xlsx updated with conclusions from training iteration 4.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3937E506-7096-4AC6-B8A2-480BB75EE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0544B-5EF0-450D-AA8F-299E1481F9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="1" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="3" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -776,9 +776,6 @@
 monitor='val_binary_accuracy'</t>
   </si>
   <si>
-    <t>Contains images from town01, town02 and town06, some images were left out from previous iteration (redudancy), as well as some labels were corrected by hand.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">0 - Vehicles </t>
     </r>
@@ -913,6 +910,27 @@
       </rPr>
       <t xml:space="preserve"> present in adjecent right lane</t>
     </r>
+  </si>
+  <si>
+    <t>Supervised/Active supervised</t>
+  </si>
+  <si>
+    <t>Contains images from town01, town02 and town06, some images were left out from previous iteration (redudancy), as well as some labels were corrected by hand.
+Gives very low acuracy on the unseen data. Network overfitted. (Validation accuracy very high because of the similirality of the images in the training set and validation set.). Problem treated as linear regression, adam optimizer, other parameters left the same as in previous iteration.</t>
+  </si>
+  <si>
+    <t>Combination of supervised/active supervised learning method applied. (Some of the images are labeled by neural network, some are labeled manually).
+Dataset correction, a lot of redudant images removed. Added images of towns 1-6, dataset shuffeled. LR optimized to 0.005. Best performance on batch size 4. Input layer changed to 200x200 (increased performance, multiple input changes took place 300x185, 300x300, 100x100). 
+Test validation accuracy performed on unseen data with threshold of 0.05 for the accurate vs. unaccurate prediction.
+The biggest challenge represents to train the last output of the neural network (CNN parameter ID-2), future changes of loss and metrics can occur due to the nature of this parameter representing three states (0, 0.5, 1)
+Model changes:
+optimizer=SGD(lr=0.005, momentum=0.9)
+loss='binary_crossentropy'
+metrics=tf.keras.metrics.CategoricalAccuracy(name="categorical_accuracy", dtype=None)
+best results with:
+batchSize=4
+ReduceLROnPlateau(factor=0.0025)
+monitor='val_binary_accuracy'</t>
   </si>
 </sst>
 </file>
@@ -950,7 +968,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -996,12 +1014,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +1126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1225,9 +1237,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1246,9 +1255,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1258,43 +1306,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1315,38 +1357,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1357,38 +1393,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3454,27 +3463,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -3483,29 +3492,29 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="60" t="s">
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="60" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="61"/>
-      <c r="S2" s="62"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="48"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -3514,29 +3523,29 @@
       <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="44" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="47" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3545,29 +3554,29 @@
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="54" t="s">
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="46" t="s">
+      <c r="P4" s="50"/>
+      <c r="Q4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
     </row>
     <row r="5" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -3576,29 +3585,29 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="54" t="s">
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="47" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -3607,29 +3616,29 @@
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="54" t="s">
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="46" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -3638,27 +3647,27 @@
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="44" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -3667,29 +3676,29 @@
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="54" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="46" t="s">
+      <c r="P8" s="50"/>
+      <c r="Q8" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -3698,27 +3707,27 @@
       <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="44" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -3727,29 +3736,29 @@
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="54" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="46" t="s">
+      <c r="P10" s="50"/>
+      <c r="Q10" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -3758,27 +3767,27 @@
       <c r="B11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="44" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -3787,29 +3796,29 @@
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="48" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="56" t="s">
+      <c r="P12" s="61"/>
+      <c r="Q12" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -3818,27 +3827,27 @@
       <c r="B13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54" t="s">
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -3847,27 +3856,27 @@
       <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="44" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
     </row>
     <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -3876,29 +3885,29 @@
       <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="44" t="s">
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="47" t="s">
+      <c r="P15" s="44"/>
+      <c r="Q15" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="R15" s="47"/>
-      <c r="S15" s="47"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -3907,29 +3916,29 @@
       <c r="B16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="44" t="s">
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="46" t="s">
+      <c r="P16" s="44"/>
+      <c r="Q16" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
     </row>
     <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -3938,29 +3947,29 @@
       <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="44" t="s">
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="47" t="s">
+      <c r="P17" s="44"/>
+      <c r="Q17" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="R17" s="47"/>
-      <c r="S17" s="47"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -3969,29 +3978,29 @@
       <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="44" t="s">
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="46" t="s">
+      <c r="P18" s="44"/>
+      <c r="Q18" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -4000,29 +4009,29 @@
       <c r="B19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54" t="s">
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="47" t="s">
+      <c r="P19" s="50"/>
+      <c r="Q19" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="R19" s="47"/>
-      <c r="S19" s="47"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -4031,29 +4040,29 @@
       <c r="B20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="54" t="s">
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="46" t="s">
+      <c r="P20" s="50"/>
+      <c r="Q20" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="R20" s="46"/>
-      <c r="S20" s="46"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
     </row>
     <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -4062,29 +4071,29 @@
       <c r="B21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="54" t="s">
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="47" t="s">
+      <c r="P21" s="50"/>
+      <c r="Q21" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -4093,29 +4102,29 @@
       <c r="B22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44" t="s">
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="46" t="s">
+      <c r="P22" s="44"/>
+      <c r="Q22" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -4124,29 +4133,29 @@
       <c r="B23" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="44" t="s">
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="47" t="s">
+      <c r="P23" s="44"/>
+      <c r="Q23" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="R23" s="47"/>
-      <c r="S23" s="47"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -4155,29 +4164,29 @@
       <c r="B24" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="48" t="s">
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="50" t="s">
+      <c r="P24" s="61"/>
+      <c r="Q24" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -4186,29 +4195,29 @@
       <c r="B25" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="44" t="s">
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="46" t="s">
+      <c r="P25" s="44"/>
+      <c r="Q25" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
     </row>
     <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -4217,32 +4226,92 @@
       <c r="B26" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="44" t="s">
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="46" t="s">
+      <c r="P26" s="44"/>
+      <c r="Q26" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="C25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="C23:N23"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
     <mergeCell ref="C26:N26"/>
     <mergeCell ref="O26:P26"/>
     <mergeCell ref="Q26:S26"/>
@@ -4259,66 +4328,6 @@
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="C14:N14"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="C25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="C23:N23"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4329,7 +4338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2E6D2C-5E3C-49D0-A2B0-F322C3268B9A}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
@@ -4341,28 +4350,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4374,29 +4383,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="61" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="77" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4408,29 +4417,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="47" t="s">
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="51" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="75"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="68"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4442,29 +4451,29 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="72" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -4476,29 +4485,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="73" t="s">
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -4510,29 +4519,29 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="57" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="72" t="s">
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -4544,29 +4553,29 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="73" t="s">
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4578,29 +4587,29 @@
       <c r="C8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="57" t="s">
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="72" t="s">
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="72"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4612,29 +4621,29 @@
       <c r="C9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="73" t="s">
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -4646,29 +4655,29 @@
       <c r="C10" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="72" t="s">
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -4748,6 +4757,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -4764,18 +4785,6 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4797,21 +4806,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4820,21 +4829,21 @@
       <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="77" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4843,19 +4852,19 @@
       <c r="B3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="75"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4864,19 +4873,19 @@
       <c r="B4" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -4885,19 +4894,19 @@
       <c r="B5" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -4906,19 +4915,19 @@
       <c r="B6" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="56">
         <v>0.25</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -4927,19 +4936,19 @@
       <c r="B7" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4948,19 +4957,19 @@
       <c r="B8" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4969,19 +4978,19 @@
       <c r="B9" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="77">
         <v>0.25</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -4990,19 +4999,19 @@
       <c r="B10" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -5011,19 +5020,19 @@
       <c r="B11" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -5032,19 +5041,19 @@
       <c r="B12" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="56">
         <v>0.25</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -5053,17 +5062,17 @@
       <c r="B13" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -5072,19 +5081,19 @@
       <c r="B14" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -5093,19 +5102,19 @@
       <c r="B15" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="67">
+      <c r="C15" s="77">
         <v>0.25</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -5114,19 +5123,19 @@
       <c r="B16" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -5135,19 +5144,19 @@
       <c r="B17" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="67">
+      <c r="C17" s="77">
         <v>0.25</v>
       </c>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -5156,19 +5165,19 @@
       <c r="B18" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -5177,24 +5186,52 @@
       <c r="B19" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="73" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M7"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="C5:H5"/>
@@ -5204,34 +5241,6 @@
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:M3"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:M18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5242,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5255,29 +5264,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5286,41 +5295,41 @@
       <c r="B2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="81" t="s">
+      <c r="D2" s="91"/>
+      <c r="E2" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="63" t="s">
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="46"/>
+      <c r="K2" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="81" t="s">
+      <c r="L2" s="92"/>
+      <c r="M2" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="91"/>
+      <c r="N2" s="93"/>
       <c r="O2" s="36" t="s">
         <v>134</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="Q2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="83"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="91"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -5334,41 +5343,41 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="84">
+      <c r="C3" s="80">
         <v>5</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="84" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="84" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="86"/>
-      <c r="K3" s="90" t="s">
+      <c r="J3" s="81"/>
+      <c r="K3" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="88"/>
-      <c r="M3" s="90" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="88"/>
+      <c r="N3" s="84"/>
       <c r="O3" s="32" t="s">
         <v>135</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="84" t="s">
+      <c r="Q3" s="80" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="86"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="81"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
@@ -5382,41 +5391,41 @@
       <c r="B4" s="21">
         <v>2321</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="56">
         <v>5</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="92" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="57">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="56">
         <v>0.97</v>
       </c>
-      <c r="J4" s="59"/>
-      <c r="K4" s="57">
+      <c r="J4" s="58"/>
+      <c r="K4" s="56">
         <v>0.96458999999999995</v>
       </c>
-      <c r="L4" s="59"/>
-      <c r="M4" s="57">
+      <c r="L4" s="58"/>
+      <c r="M4" s="56">
         <v>0.94051739999999995</v>
       </c>
-      <c r="N4" s="59"/>
+      <c r="N4" s="58"/>
       <c r="O4" s="21" t="s">
         <v>137</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="57" t="s">
+      <c r="Q4" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="59"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="58"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
@@ -5430,71 +5439,89 @@
       <c r="B5" s="23">
         <v>2048</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="80">
         <v>5</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="84" t="s">
+      <c r="D5" s="81"/>
+      <c r="E5" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="86"/>
-      <c r="K5" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="L5" s="88"/>
-      <c r="M5" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" s="88"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="80">
+        <v>0.96</v>
+      </c>
+      <c r="J5" s="81"/>
+      <c r="K5" s="80">
+        <v>0.96</v>
+      </c>
+      <c r="L5" s="84"/>
+      <c r="M5" s="80">
+        <v>0.6</v>
+      </c>
+      <c r="N5" s="84"/>
       <c r="O5" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="P5" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="84" t="s">
-        <v>140</v>
-      </c>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="86"/>
+      <c r="P5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="80" t="s">
+        <v>146</v>
+      </c>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="81"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="59"/>
+      <c r="B6" s="21">
+        <v>1798</v>
+      </c>
+      <c r="C6" s="56">
+        <v>5</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="56">
+        <v>0.75</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="L6" s="58"/>
+      <c r="M6" s="56">
+        <v>0.88715080000000002</v>
+      </c>
+      <c r="N6" s="58"/>
+      <c r="O6" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="58"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -5506,18 +5533,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="88"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="84"/>
       <c r="O7" s="35"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="19"/>
@@ -5536,25 +5563,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="59"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="58"/>
       <c r="O8" s="21"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="59"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="58"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -5566,18 +5593,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="88"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="84"/>
       <c r="O9" s="35"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19"/>
@@ -5596,43 +5623,43 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="59"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="58"/>
       <c r="O10" s="21"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="59"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="58"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="88"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="84"/>
       <c r="O11" s="35"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="19"/>
@@ -5646,25 +5673,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="59"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="58"/>
       <c r="O12" s="21"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="59"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="58"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -5734,6 +5761,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="Q10:U10"/>
@@ -5750,54 +5825,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dataset_additional_part_1.csv completely labeled backup. Additional changes to some of the scripts regarding model loading.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0544B-5EF0-450D-AA8F-299E1481F9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CC05F3-863C-4F21-8F1B-7159BC5FDFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="3" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" firstSheet="1" activeTab="5" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CNN architecture overview" sheetId="4" r:id="rId3"/>
     <sheet name="CNN training overview" sheetId="3" r:id="rId4"/>
     <sheet name="Dataset collection process" sheetId="5" r:id="rId5"/>
+    <sheet name="General notes" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="153">
   <si>
     <t>Safe to accelerate</t>
   </si>
@@ -647,9 +648,6 @@
     <t>Input layer</t>
   </si>
   <si>
-    <t>100x100</t>
-  </si>
-  <si>
     <t>Conv2D(16, (3,3), activation= 'relu')</t>
   </si>
   <si>
@@ -919,8 +917,11 @@
 Gives very low acuracy on the unseen data. Network overfitted. (Validation accuracy very high because of the similirality of the images in the training set and validation set.). Problem treated as linear regression, adam optimizer, other parameters left the same as in previous iteration.</t>
   </si>
   <si>
+    <t>200x200</t>
+  </si>
+  <si>
     <t>Combination of supervised/active supervised learning method applied. (Some of the images are labeled by neural network, some are labeled manually).
-Dataset correction, a lot of redudant images removed. Added images of towns 1-6, dataset shuffeled. LR optimized to 0.005. Best performance on batch size 4. Input layer changed to 200x200 (increased performance, multiple input changes took place 300x185, 300x300, 100x100). 
+Dataset correction, a lot of redudant images removed. Added images of towns 1-6, dataset shuffeled. LR optimized to 0.005. Best performance on batch size 2. Input layer changed to 200x200 (increased performance, multiple input changes took place 300x185, 300x300, 100x100). 
 Test validation accuracy performed on unseen data with threshold of 0.05 for the accurate vs. unaccurate prediction.
 The biggest challenge represents to train the last output of the neural network (CNN parameter ID-2), future changes of loss and metrics can occur due to the nature of this parameter representing three states (0, 0.5, 1)
 Model changes:
@@ -928,9 +929,29 @@
 loss='binary_crossentropy'
 metrics=tf.keras.metrics.CategoricalAccuracy(name="categorical_accuracy", dtype=None)
 best results with:
-batchSize=4
+batchSize=2
 ReduceLROnPlateau(factor=0.0025)
 monitor='val_binary_accuracy'</t>
+  </si>
+  <si>
+    <t>General notes</t>
+  </si>
+  <si>
+    <t>Outputs of the YOLOv3 neural network can be used as a verification criteria (comaprison criteria) for the outputs of the CNN that mark the probabilities that there are vehicles present on the input frame.</t>
+  </si>
+  <si>
+    <t>The system can be constrained to work only up to certain speeds (e.g. 80km/h) and thus trained in a manner of maximal speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety mechanism can be introduced into the system where it will take over the control of the ego vehicle if it is observed that the CNN does not slow down the car in certain situtations. This would impose emergency braking system in procedural manner thus creating fully functional simplified system. </t>
+  </si>
+  <si>
+    <t>Possible scenario ideas:
+1) Empty road
+2) Ego vehicle coming to ongoing traffic
+3) Ego vehicle in the middle of ongoing traffic
+4) Ego vehicle coming to stopped traffic
+5) Vehicles cutting off ego vehicle in ongoing traffic</t>
   </si>
 </sst>
 </file>
@@ -1255,55 +1276,73 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1339,38 +1378,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1380,24 +1419,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3463,27 +3484,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -3492,29 +3513,29 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="47" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="47" t="s">
+      <c r="P2" s="61"/>
+      <c r="Q2" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="48"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="61"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -3523,29 +3544,29 @@
       <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P3" s="44"/>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3568,10 +3589,10 @@
       <c r="L4" s="57"/>
       <c r="M4" s="57"/>
       <c r="N4" s="58"/>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="50"/>
+      <c r="P4" s="54"/>
       <c r="Q4" s="45" t="s">
         <v>39</v>
       </c>
@@ -3585,29 +3606,29 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="49" t="s">
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="52" t="s">
+      <c r="P5" s="54"/>
+      <c r="Q5" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -3630,10 +3651,10 @@
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
       <c r="N6" s="42"/>
-      <c r="O6" s="49" t="s">
+      <c r="O6" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="50"/>
+      <c r="P6" s="54"/>
       <c r="Q6" s="45" t="s">
         <v>108</v>
       </c>
@@ -3647,27 +3668,27 @@
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="52"/>
       <c r="O7" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P7" s="44"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -3690,10 +3711,10 @@
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="50"/>
+      <c r="P8" s="54"/>
       <c r="Q8" s="45" t="s">
         <v>82</v>
       </c>
@@ -3707,27 +3728,27 @@
       <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="55"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="52"/>
       <c r="O9" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P9" s="44"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -3750,10 +3771,10 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="42"/>
-      <c r="O10" s="49" t="s">
+      <c r="O10" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="50"/>
+      <c r="P10" s="54"/>
       <c r="Q10" s="45" t="s">
         <v>44</v>
       </c>
@@ -3767,27 +3788,27 @@
       <c r="B11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="55"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="52"/>
       <c r="O11" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P11" s="44"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -3810,11 +3831,11 @@
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="42"/>
-      <c r="O12" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="59" t="s">
+      <c r="O12" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="55" t="s">
         <v>49</v>
       </c>
       <c r="R12" s="45"/>
@@ -3827,27 +3848,27 @@
       <c r="B13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="49" t="s">
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -3885,29 +3906,29 @@
       <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="55"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="52"/>
       <c r="O15" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P15" s="44"/>
-      <c r="Q15" s="52" t="s">
+      <c r="Q15" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="R15" s="52"/>
-      <c r="S15" s="52"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -3947,29 +3968,29 @@
       <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="55"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="52"/>
       <c r="O17" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P17" s="44"/>
-      <c r="Q17" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
+      <c r="Q17" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -4009,29 +4030,29 @@
       <c r="B19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="49" t="s">
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="52" t="s">
+      <c r="P19" s="54"/>
+      <c r="Q19" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="R19" s="52"/>
-      <c r="S19" s="52"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -4054,10 +4075,10 @@
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
       <c r="N20" s="42"/>
-      <c r="O20" s="49" t="s">
+      <c r="O20" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P20" s="50"/>
+      <c r="P20" s="54"/>
       <c r="Q20" s="45" t="s">
         <v>73</v>
       </c>
@@ -4071,29 +4092,29 @@
       <c r="B21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="49" t="s">
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="52" t="s">
+      <c r="P21" s="54"/>
+      <c r="Q21" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="R21" s="52"/>
-      <c r="S21" s="52"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -4133,29 +4154,29 @@
       <c r="B23" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="55"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="52"/>
       <c r="O23" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P23" s="44"/>
-      <c r="Q23" s="52" t="s">
+      <c r="Q23" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="R23" s="52"/>
-      <c r="S23" s="52"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -4178,11 +4199,11 @@
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
       <c r="N24" s="42"/>
-      <c r="O24" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="62" t="s">
+      <c r="O24" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="49" t="s">
         <v>101</v>
       </c>
       <c r="R24" s="45"/>
@@ -4193,10 +4214,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="40" t="s">
         <v>125</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>126</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
@@ -4214,7 +4235,7 @@
       </c>
       <c r="P25" s="44"/>
       <c r="Q25" s="45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R25" s="45"/>
       <c r="S25" s="45"/>
@@ -4224,10 +4245,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>129</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>130</v>
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
@@ -4245,13 +4266,73 @@
       </c>
       <c r="P26" s="44"/>
       <c r="Q26" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R26" s="45"/>
       <c r="S26" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="C26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
     <mergeCell ref="C25:N25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:S25"/>
@@ -4268,66 +4349,6 @@
     <mergeCell ref="C23:N23"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="C26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="C14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4350,28 +4371,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4383,29 +4404,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="51" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="70" t="s">
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4417,29 +4438,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="52" t="s">
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="68"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="74"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4460,20 +4481,20 @@
       <c r="H4" s="41"/>
       <c r="I4" s="42"/>
       <c r="J4" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K4" s="57"/>
       <c r="L4" s="57"/>
       <c r="M4" s="57"/>
       <c r="N4" s="57"/>
       <c r="O4" s="58"/>
-      <c r="P4" s="65" t="s">
+      <c r="P4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -4485,29 +4506,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="66" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -4535,13 +4556,13 @@
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
       <c r="O6" s="58"/>
-      <c r="P6" s="65" t="s">
+      <c r="P6" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -4553,29 +4574,29 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="66" t="s">
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
-      <c r="T7" s="66"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
+      <c r="S7" s="72"/>
+      <c r="T7" s="72"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4603,13 +4624,13 @@
       <c r="M8" s="57"/>
       <c r="N8" s="57"/>
       <c r="O8" s="58"/>
-      <c r="P8" s="65" t="s">
+      <c r="P8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4621,29 +4642,29 @@
       <c r="C9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="66" t="s">
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="72"/>
+      <c r="T9" s="72"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -4664,20 +4685,20 @@
       <c r="H10" s="41"/>
       <c r="I10" s="42"/>
       <c r="J10" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K10" s="57"/>
       <c r="L10" s="57"/>
       <c r="M10" s="57"/>
       <c r="N10" s="57"/>
       <c r="O10" s="58"/>
-      <c r="P10" s="65" t="s">
+      <c r="P10" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -4757,18 +4778,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -4785,6 +4794,18 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4797,7 +4818,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:M19"/>
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4806,21 +4827,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4829,21 +4850,21 @@
       <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="70" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4852,68 +4873,68 @@
       <c r="B3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="68"/>
+      <c r="C3" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="74"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="57"/>
       <c r="F4" s="57"/>
       <c r="G4" s="57"/>
       <c r="H4" s="58"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="56">
         <v>0.25</v>
@@ -4923,123 +4944,123 @@
       <c r="F6" s="57"/>
       <c r="G6" s="57"/>
       <c r="H6" s="58"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
+        <v>119</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="56" t="s">
         <v>113</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>114</v>
       </c>
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
       <c r="F8" s="57"/>
       <c r="G8" s="57"/>
       <c r="H8" s="58"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="77">
+        <v>114</v>
+      </c>
+      <c r="C9" s="66">
         <v>0.25</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="57"/>
       <c r="E10" s="57"/>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="56">
         <v>0.25</v>
@@ -5049,189 +5070,161 @@
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="58"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
+        <v>117</v>
+      </c>
+      <c r="C13" s="66"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
       <c r="F14" s="57"/>
       <c r="G14" s="57"/>
       <c r="H14" s="58"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="77">
+        <v>114</v>
+      </c>
+      <c r="C15" s="66">
         <v>0.25</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="57"/>
       <c r="E16" s="57"/>
       <c r="F16" s="57"/>
       <c r="G16" s="57"/>
       <c r="H16" s="58"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="77">
+        <v>114</v>
+      </c>
+      <c r="C17" s="66">
         <v>0.25</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18" s="57"/>
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="57"/>
       <c r="H18" s="58"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="71"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="77" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="J19" s="66"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="66"/>
+        <v>118</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M7"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="C5:H5"/>
@@ -5241,6 +5234,34 @@
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:M3"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5251,8 +5272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E76F5-A85A-4895-850D-166481800471}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5264,29 +5285,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5295,41 +5316,41 @@
       <c r="B2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="89" t="s">
+      <c r="D2" s="82"/>
+      <c r="E2" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="46" t="s">
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46" t="s">
+      <c r="J2" s="62"/>
+      <c r="K2" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="L2" s="92"/>
-      <c r="M2" s="89" t="s">
+      <c r="L2" s="88"/>
+      <c r="M2" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="93"/>
+      <c r="N2" s="90"/>
       <c r="O2" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="89" t="s">
+      <c r="Q2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="91"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="82"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -5343,41 +5364,41 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="83">
         <v>5</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="85"/>
+      <c r="E3" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="80" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="81"/>
-      <c r="K3" s="82" t="s">
+      <c r="J3" s="85"/>
+      <c r="K3" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="84"/>
-      <c r="M3" s="82" t="s">
+      <c r="L3" s="87"/>
+      <c r="M3" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="84"/>
+      <c r="N3" s="87"/>
       <c r="O3" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88"/>
-      <c r="U3" s="81"/>
+      <c r="Q3" s="83" t="s">
+        <v>135</v>
+      </c>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="85"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
@@ -5395,12 +5416,12 @@
         <v>5</v>
       </c>
       <c r="D4" s="58"/>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="87"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="56">
         <v>0.97</v>
       </c>
@@ -5414,13 +5435,13 @@
       </c>
       <c r="N4" s="58"/>
       <c r="O4" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>23</v>
       </c>
       <c r="Q4" s="56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R4" s="57"/>
       <c r="S4" s="57"/>
@@ -5439,41 +5460,41 @@
       <c r="B5" s="23">
         <v>2048</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="83">
         <v>5</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="80" t="s">
+      <c r="D5" s="85"/>
+      <c r="E5" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="80">
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="83">
         <v>0.96</v>
       </c>
-      <c r="J5" s="81"/>
-      <c r="K5" s="80">
+      <c r="J5" s="85"/>
+      <c r="K5" s="83">
         <v>0.96</v>
       </c>
-      <c r="L5" s="84"/>
-      <c r="M5" s="80">
+      <c r="L5" s="87"/>
+      <c r="M5" s="83">
         <v>0.6</v>
       </c>
-      <c r="N5" s="84"/>
+      <c r="N5" s="87"/>
       <c r="O5" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="80" t="s">
-        <v>146</v>
-      </c>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="81"/>
+      <c r="Q5" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="R5" s="84"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="84"/>
+      <c r="U5" s="85"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
@@ -5491,12 +5512,12 @@
         <v>5</v>
       </c>
       <c r="D6" s="58"/>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="87"/>
       <c r="I6" s="56">
         <v>0.75</v>
       </c>
@@ -5510,7 +5531,7 @@
       </c>
       <c r="N6" s="58"/>
       <c r="O6" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>23</v>
@@ -5533,18 +5554,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="84"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="87"/>
       <c r="O7" s="35"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="19"/>
@@ -5593,18 +5614,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="84"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="87"/>
       <c r="O9" s="35"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19"/>
@@ -5648,18 +5669,18 @@
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="84"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="87"/>
       <c r="O11" s="35"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="19"/>
@@ -5761,6 +5782,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="Q10:U10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="Q5:U5"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="Q2:U2"/>
@@ -5777,54 +5846,6 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5844,4 +5865,315 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4962BCEB-1AB5-4BD5-AA16-39B026A7DD7F}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="58"/>
+    </row>
+    <row r="4" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="68"/>
+    </row>
+    <row r="5" spans="1:21" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="58"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="68"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="58"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="66"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="68"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="58"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="66"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="67"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="68"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="B11:U11"/>
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="B3:U3"/>
+    <mergeCell ref="B4:U4"/>
+    <mergeCell ref="B5:U5"/>
+    <mergeCell ref="B6:U6"/>
+    <mergeCell ref="B7:U7"/>
+    <mergeCell ref="B8:U8"/>
+    <mergeCell ref="B9:U9"/>
+    <mergeCell ref="B10:U10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MainSimulation.py spawnScenarioVehicles function added for spawning traffic participants. 3 Scenarios added - empty road, ongoing traffic with leading vehicle, ongoing traffic without leading vehicle. Scenario switching WIP.
</commit_message>
<xml_diff>
--- a/doc/system_overview.xlsx
+++ b/doc/system_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\CARLA_0_9_12\WindowsNoEditor\PythonAPI\ADAS-ML-DistanceKeeping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0416DC4-11EF-4B85-A17F-047BF3E13399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBCF3FE-53F8-4725-8897-E148D680D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" firstSheet="1" activeTab="5" xr2:uid="{6121A5D0-839D-4329-8C00-F539DE4428B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional overview" sheetId="2" r:id="rId1"/>
@@ -895,14 +895,6 @@
     <t xml:space="preserve">Safety mechanism can be introduced into the system where it will take over the control of the ego vehicle if it is observed that the CNN does not slow down the car in certain situtations. This would impose emergency braking system in procedural manner thus creating fully functional simplified system. </t>
   </si>
   <si>
-    <t>Possible scenario ideas:
-1) Empty road
-2) Ego vehicle coming to ongoing traffic
-3) Ego vehicle in the middle of ongoing traffic
-4) Ego vehicle coming to stopped traffic
-5) Vehicles cutting off ego vehicle in ongoing traffic</t>
-  </si>
-  <si>
     <t>The system shall determine if there is a leading vehicle In the lane of the driving vehicle based on the outputs of CNN.</t>
   </si>
   <si>
@@ -942,6 +934,15 @@
   </si>
   <si>
     <t>Based on the possibilities of CARLA simulator. Possible scenarios in the General notes tab</t>
+  </si>
+  <si>
+    <t>Possible scenario ideas:
+1) Empty road
+2) Ego vehicle coming to ongoing traffic
+3) Ego vehicle in the middle of ongoing traffic
+4) Ego vehicle coming to stopped traffic
+5) Vehicles cutting off ego vehicle in ongoing traffic
+6) No leading vehicle</t>
   </si>
 </sst>
 </file>
@@ -1266,9 +1267,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1278,43 +1318,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,38 +1369,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1377,38 +1405,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3460,8 +3461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057AB9DD-F128-4D99-8970-0A2CE814DFB4}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21:P21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,27 +3475,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -3503,29 +3504,29 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="59" t="s">
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="59" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="61"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="48"/>
     </row>
     <row r="3" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -3534,29 +3535,29 @@
       <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="55"/>
       <c r="O3" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P3" s="44"/>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
     </row>
     <row r="4" spans="1:19" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3579,12 +3580,12 @@
       <c r="L4" s="57"/>
       <c r="M4" s="57"/>
       <c r="N4" s="58"/>
-      <c r="O4" s="53" t="s">
+      <c r="O4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="54"/>
+      <c r="P4" s="50"/>
       <c r="Q4" s="45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R4" s="45"/>
       <c r="S4" s="45"/>
@@ -3596,29 +3597,29 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
+      <c r="C5" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
       <c r="O5" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P5" s="44"/>
-      <c r="Q5" s="46" t="s">
+      <c r="Q5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -3658,27 +3659,27 @@
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
+      <c r="C7" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
       <c r="O7" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P7" s="44"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -3701,10 +3702,10 @@
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="53" t="s">
+      <c r="O8" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="54"/>
+      <c r="P8" s="50"/>
       <c r="Q8" s="45" t="s">
         <v>77</v>
       </c>
@@ -3718,27 +3719,27 @@
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="52"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="55"/>
       <c r="O9" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P9" s="44"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -3761,12 +3762,12 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="42"/>
-      <c r="O10" s="53" t="s">
+      <c r="O10" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="54"/>
+      <c r="P10" s="50"/>
       <c r="Q10" s="45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R10" s="45"/>
       <c r="S10" s="45"/>
@@ -3778,29 +3779,29 @@
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="52"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
       <c r="O11" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P11" s="44"/>
-      <c r="Q11" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
+      <c r="Q11" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -3823,11 +3824,11 @@
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="42"/>
-      <c r="O12" s="47" t="s">
+      <c r="O12" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="55" t="s">
+      <c r="P12" s="61"/>
+      <c r="Q12" s="59" t="s">
         <v>46</v>
       </c>
       <c r="R12" s="45"/>
@@ -3840,27 +3841,27 @@
       <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="53" t="s">
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -3898,29 +3899,29 @@
       <c r="B15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="52"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="55"/>
       <c r="O15" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P15" s="44"/>
-      <c r="Q15" s="46" t="s">
+      <c r="Q15" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="R15" s="46"/>
-      <c r="S15" s="46"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
     </row>
     <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -3960,29 +3961,29 @@
       <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="52"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="55"/>
       <c r="O17" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P17" s="44"/>
-      <c r="Q17" s="46" t="s">
+      <c r="Q17" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -4022,29 +4023,29 @@
       <c r="B19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="52"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="55"/>
       <c r="O19" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P19" s="44"/>
-      <c r="Q19" s="46" t="s">
+      <c r="Q19" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -4084,29 +4085,29 @@
       <c r="B21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52"/>
+      <c r="C21" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
       <c r="O21" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P21" s="44"/>
-      <c r="Q21" s="46" t="s">
+      <c r="Q21" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
     </row>
     <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -4146,29 +4147,29 @@
       <c r="B23" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="52"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="55"/>
       <c r="O23" s="43" t="s">
         <v>23</v>
       </c>
       <c r="P23" s="44"/>
-      <c r="Q23" s="46" t="s">
+      <c r="Q23" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
     </row>
     <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -4191,11 +4192,11 @@
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
       <c r="N24" s="42"/>
-      <c r="O24" s="47" t="s">
+      <c r="O24" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="49" t="s">
+      <c r="P24" s="61"/>
+      <c r="Q24" s="62" t="s">
         <v>96</v>
       </c>
       <c r="R24" s="45"/>
@@ -4265,6 +4266,66 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="C25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="C23:N23"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
     <mergeCell ref="C26:N26"/>
     <mergeCell ref="O26:P26"/>
     <mergeCell ref="Q26:S26"/>
@@ -4281,66 +4342,6 @@
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="C14:N14"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="C25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="C23:N23"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4363,28 +4364,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4396,29 +4397,29 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="60" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="76" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4430,29 +4431,29 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="46" t="s">
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="50" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="74"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="68"/>
     </row>
     <row r="4" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4480,13 +4481,13 @@
       <c r="M4" s="57"/>
       <c r="N4" s="57"/>
       <c r="O4" s="58"/>
-      <c r="P4" s="71" t="s">
+      <c r="P4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
     </row>
     <row r="5" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -4498,29 +4499,29 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66" t="s">
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="72" t="s">
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
     </row>
     <row r="6" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -4548,13 +4549,13 @@
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
       <c r="O6" s="58"/>
-      <c r="P6" s="71" t="s">
+      <c r="P6" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
     </row>
     <row r="7" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -4566,29 +4567,29 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="66" t="s">
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="72" t="s">
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="72"/>
-      <c r="S7" s="72"/>
-      <c r="T7" s="72"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
     </row>
     <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4616,13 +4617,13 @@
       <c r="M8" s="57"/>
       <c r="N8" s="57"/>
       <c r="O8" s="58"/>
-      <c r="P8" s="71" t="s">
+      <c r="P8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="71"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4634,29 +4635,29 @@
       <c r="C9" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="66" t="s">
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="72" t="s">
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="Q9" s="72"/>
-      <c r="R9" s="72"/>
-      <c r="S9" s="72"/>
-      <c r="T9" s="72"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -4684,13 +4685,13 @@
       <c r="M10" s="57"/>
       <c r="N10" s="57"/>
       <c r="O10" s="58"/>
-      <c r="P10" s="71" t="s">
+      <c r="P10" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="71"/>
-      <c r="T10" s="71"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
@@ -4770,6 +4771,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="P8:T8"/>
@@ -4786,18 +4799,6 @@
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4819,21 +4820,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4842,21 +4843,21 @@
       <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="76" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -4865,19 +4866,19 @@
       <c r="B3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="74"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4894,11 +4895,11 @@
       <c r="F4" s="57"/>
       <c r="G4" s="57"/>
       <c r="H4" s="58"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -4907,19 +4908,19 @@
       <c r="B5" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -4936,11 +4937,11 @@
       <c r="F6" s="57"/>
       <c r="G6" s="57"/>
       <c r="H6" s="58"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -4949,19 +4950,19 @@
       <c r="B7" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -4978,11 +4979,11 @@
       <c r="F8" s="57"/>
       <c r="G8" s="57"/>
       <c r="H8" s="58"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -4991,19 +4992,19 @@
       <c r="B9" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="66">
+      <c r="C9" s="77">
         <v>0.25</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -5020,11 +5021,11 @@
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -5033,19 +5034,19 @@
       <c r="B11" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -5062,11 +5063,11 @@
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="58"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -5075,17 +5076,17 @@
       <c r="B13" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -5102,11 +5103,11 @@
       <c r="F14" s="57"/>
       <c r="G14" s="57"/>
       <c r="H14" s="58"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -5115,19 +5116,19 @@
       <c r="B15" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="66">
+      <c r="C15" s="77">
         <v>0.25</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -5144,11 +5145,11 @@
       <c r="F16" s="57"/>
       <c r="G16" s="57"/>
       <c r="H16" s="58"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -5157,19 +5158,19 @@
       <c r="B17" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="66">
+      <c r="C17" s="77">
         <v>0.25</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -5186,11 +5187,11 @@
       <c r="F18" s="57"/>
       <c r="G18" s="57"/>
       <c r="H18" s="58"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -5199,24 +5200,52 @@
       <c r="B19" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="72" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:M7"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="C5:H5"/>
@@ -5226,34 +5255,6 @@
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:M3"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:M18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5277,29 +5278,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5308,41 +5309,41 @@
       <c r="B2" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="80" t="s">
+      <c r="D2" s="91"/>
+      <c r="E2" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="62" t="s">
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="46"/>
+      <c r="K2" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="88"/>
-      <c r="M2" s="80" t="s">
+      <c r="L2" s="92"/>
+      <c r="M2" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="90"/>
+      <c r="N2" s="93"/>
       <c r="O2" s="36" t="s">
         <v>128</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="Q2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="82"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="91"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -5356,41 +5357,41 @@
       <c r="B3" s="13">
         <v>1218</v>
       </c>
-      <c r="C3" s="83">
+      <c r="C3" s="80">
         <v>5</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="83" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="83" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="85"/>
-      <c r="K3" s="89" t="s">
+      <c r="J3" s="81"/>
+      <c r="K3" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="M3" s="89" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="87"/>
+      <c r="N3" s="84"/>
       <c r="O3" s="32" t="s">
         <v>129</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="83" t="s">
+      <c r="Q3" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="85"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="81"/>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
@@ -5408,12 +5409,12 @@
         <v>5</v>
       </c>
       <c r="D4" s="58"/>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
       <c r="I4" s="56">
         <v>0.97</v>
       </c>
@@ -5452,41 +5453,41 @@
       <c r="B5" s="23">
         <v>2048</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="80">
         <v>5</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="83" t="s">
+      <c r="D5" s="81"/>
+      <c r="E5" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="83">
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="80">
         <v>0.96</v>
       </c>
-      <c r="J5" s="85"/>
-      <c r="K5" s="83">
+      <c r="J5" s="81"/>
+      <c r="K5" s="80">
         <v>0.96</v>
       </c>
-      <c r="L5" s="87"/>
-      <c r="M5" s="83">
+      <c r="L5" s="84"/>
+      <c r="M5" s="80">
         <v>0.6</v>
       </c>
-      <c r="N5" s="87"/>
+      <c r="N5" s="84"/>
       <c r="O5" s="38" t="s">
         <v>131</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="83" t="s">
+      <c r="Q5" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="R5" s="84"/>
-      <c r="S5" s="84"/>
-      <c r="T5" s="84"/>
-      <c r="U5" s="85"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="81"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
@@ -5504,12 +5505,12 @@
         <v>5</v>
       </c>
       <c r="D6" s="58"/>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="87"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="56">
         <v>0.75</v>
       </c>
@@ -5546,18 +5547,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="87"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="84"/>
       <c r="O7" s="35"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="19"/>
@@ -5606,18 +5607,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="87"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="84"/>
       <c r="O9" s="35"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19"/>
@@ -5661,18 +5662,18 @@
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="87"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="87"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="84"/>
       <c r="O11" s="35"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="19"/>
@@ -5774,6 +5775,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="Q10:U10"/>
@@ -5790,54 +5839,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5863,63 +5864,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4962BCEB-1AB5-4BD5-AA16-39B026A7DD7F}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="81"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
@@ -5952,35 +5953,35 @@
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="79"/>
     </row>
     <row r="5" spans="1:21" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
@@ -6006,26 +6007,26 @@
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="68"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="79"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -6056,26 +6057,26 @@
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="67"/>
-      <c r="U8" s="68"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="79"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -6106,26 +6107,26 @@
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="68"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="78"/>
+      <c r="T10" s="78"/>
+      <c r="U10" s="79"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="9">

</xml_diff>